<commit_message>
Update my Gantt chart -- coding standards
</commit_message>
<xml_diff>
--- a/Documents/Master Gantt.xlsx
+++ b/Documents/Master Gantt.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10123"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BenjaminHallman/Documents/College/Classes/Computer Science/383/Projects/Dream Team/Project Manager/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Delaney/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D7C555-7F0F-B34D-91F9-1F7049444D37}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Management Summary" sheetId="3" r:id="rId1"/>
@@ -18,9 +17,15 @@
     <sheet name="Meetings" sheetId="2" r:id="rId3"/>
     <sheet name="SA" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="42">
   <si>
     <t>group totals (hrs)</t>
   </si>
@@ -167,16 +172,19 @@
   <si>
     <t>Master Gantt Chart</t>
   </si>
+  <si>
+    <t xml:space="preserve">Coding Standards </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,11 +285,11 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -290,7 +298,7 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -298,17 +306,17 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -318,7 +326,7 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -326,12 +334,12 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -340,31 +348,31 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -372,23 +380,23 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -427,15 +435,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -536,6 +535,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -849,14 +857,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
@@ -876,427 +884,427 @@
     <col min="16" max="16" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
-      <c r="B1" s="28" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B1" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="30"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="66"/>
       <c r="E1" s="8"/>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="29"/>
-      <c r="H1" s="30"/>
-      <c r="J1" s="28" t="s">
+      <c r="G1" s="65"/>
+      <c r="H1" s="66"/>
+      <c r="J1" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="29"/>
-      <c r="L1" s="30"/>
-      <c r="N1" s="28" t="s">
+      <c r="K1" s="65"/>
+      <c r="L1" s="66"/>
+      <c r="N1" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="29"/>
-      <c r="P1" s="30"/>
-    </row>
-    <row r="2" spans="1:16" ht="16" thickBot="1">
-      <c r="B2" s="42" t="s">
+      <c r="O1" s="65"/>
+      <c r="P1" s="66"/>
+    </row>
+    <row r="2" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="45"/>
-      <c r="F2" s="46" t="s">
+      <c r="E2" s="42"/>
+      <c r="F2" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="47" t="s">
+      <c r="G2" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="48" t="s">
+      <c r="H2" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="49"/>
-      <c r="J2" s="46" t="s">
+      <c r="I2" s="46"/>
+      <c r="J2" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="47" t="s">
+      <c r="K2" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="48" t="s">
+      <c r="L2" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="49"/>
-      <c r="N2" s="42" t="s">
+      <c r="M2" s="46"/>
+      <c r="N2" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="43" t="s">
+      <c r="O2" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="44" t="s">
+      <c r="P2" s="41" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="50">
-        <v>0</v>
-      </c>
-      <c r="C3" s="51">
-        <v>0</v>
-      </c>
-      <c r="D3" s="52">
+      <c r="B3" s="47">
+        <v>0</v>
+      </c>
+      <c r="C3" s="48">
+        <v>0</v>
+      </c>
+      <c r="D3" s="49">
         <f>(B3-C3)</f>
         <v>0</v>
       </c>
-      <c r="E3" s="45"/>
-      <c r="F3" s="53">
+      <c r="E3" s="42"/>
+      <c r="F3" s="50">
         <f>(Gantt!$B10)*100</f>
         <v>0</v>
       </c>
-      <c r="G3" s="54">
+      <c r="G3" s="51">
         <f>(Gantt!$C10)*100</f>
         <v>0</v>
       </c>
-      <c r="H3" s="55">
+      <c r="H3" s="52">
         <f>(F3-G3)</f>
         <v>0</v>
       </c>
-      <c r="I3" s="49"/>
-      <c r="J3" s="50">
-        <v>0</v>
-      </c>
-      <c r="K3" s="51">
+      <c r="I3" s="46"/>
+      <c r="J3" s="47">
+        <v>0</v>
+      </c>
+      <c r="K3" s="48">
         <f>Meetings!B4*100</f>
         <v>150</v>
       </c>
-      <c r="L3" s="52">
+      <c r="L3" s="49">
         <f>(J3-K3)</f>
         <v>-150</v>
       </c>
-      <c r="M3" s="49"/>
-      <c r="N3" s="50">
-        <v>0</v>
-      </c>
-      <c r="O3" s="51">
-        <v>0</v>
-      </c>
-      <c r="P3" s="52">
+      <c r="M3" s="46"/>
+      <c r="N3" s="47">
+        <v>0</v>
+      </c>
+      <c r="O3" s="48">
+        <v>0</v>
+      </c>
+      <c r="P3" s="49">
         <f>(N3-O3)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="53">
-        <v>0</v>
-      </c>
-      <c r="C4" s="54">
-        <v>0</v>
-      </c>
-      <c r="D4" s="55">
+      <c r="B4" s="50">
+        <v>0</v>
+      </c>
+      <c r="C4" s="51">
+        <v>0</v>
+      </c>
+      <c r="D4" s="52">
         <f t="shared" ref="D4:D5" si="0">(B4-C4)</f>
         <v>0</v>
       </c>
-      <c r="E4" s="45"/>
-      <c r="F4" s="53">
+      <c r="E4" s="42"/>
+      <c r="F4" s="50">
         <f>(Gantt!$B18)*100</f>
         <v>0</v>
       </c>
-      <c r="G4" s="54">
+      <c r="G4" s="51">
         <f>(Gantt!$C18)*100</f>
         <v>0</v>
       </c>
-      <c r="H4" s="55">
+      <c r="H4" s="52">
         <f t="shared" ref="H4:H5" si="1">(F4-G4)</f>
         <v>0</v>
       </c>
-      <c r="I4" s="49"/>
-      <c r="J4" s="53">
-        <v>0</v>
-      </c>
-      <c r="K4" s="54">
-        <v>0</v>
-      </c>
-      <c r="L4" s="55">
+      <c r="I4" s="46"/>
+      <c r="J4" s="50">
+        <v>0</v>
+      </c>
+      <c r="K4" s="51">
+        <v>0</v>
+      </c>
+      <c r="L4" s="52">
         <f t="shared" ref="L4:L5" si="2">(J4-K4)</f>
         <v>0</v>
       </c>
-      <c r="M4" s="49"/>
-      <c r="N4" s="53">
-        <v>0</v>
-      </c>
-      <c r="O4" s="54">
-        <v>0</v>
-      </c>
-      <c r="P4" s="55">
+      <c r="M4" s="46"/>
+      <c r="N4" s="50">
+        <v>0</v>
+      </c>
+      <c r="O4" s="51">
+        <v>0</v>
+      </c>
+      <c r="P4" s="52">
         <f t="shared" ref="P4:P5" si="3">(N4-O4)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="53">
-        <v>0</v>
-      </c>
-      <c r="C5" s="54">
-        <v>0</v>
-      </c>
-      <c r="D5" s="55">
+      <c r="B5" s="50">
+        <v>0</v>
+      </c>
+      <c r="C5" s="51">
+        <v>0</v>
+      </c>
+      <c r="D5" s="52">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E5" s="45"/>
-      <c r="F5" s="53">
+      <c r="E5" s="42"/>
+      <c r="F5" s="50">
         <f>(Gantt!$B26)*100</f>
         <v>0</v>
       </c>
-      <c r="G5" s="54">
+      <c r="G5" s="51">
         <f>(Gantt!$C26)*100</f>
         <v>0</v>
       </c>
-      <c r="H5" s="55">
+      <c r="H5" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I5" s="49"/>
-      <c r="J5" s="53">
-        <v>0</v>
-      </c>
-      <c r="K5" s="54">
+      <c r="I5" s="46"/>
+      <c r="J5" s="50">
+        <v>0</v>
+      </c>
+      <c r="K5" s="51">
         <f>Meetings!B4*100</f>
         <v>150</v>
       </c>
-      <c r="L5" s="55">
+      <c r="L5" s="52">
         <f t="shared" si="2"/>
         <v>-150</v>
       </c>
-      <c r="M5" s="49"/>
-      <c r="N5" s="53">
-        <v>0</v>
-      </c>
-      <c r="O5" s="54">
-        <v>0</v>
-      </c>
-      <c r="P5" s="55">
+      <c r="M5" s="46"/>
+      <c r="N5" s="50">
+        <v>0</v>
+      </c>
+      <c r="O5" s="51">
+        <v>0</v>
+      </c>
+      <c r="P5" s="52">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="53">
-        <v>0</v>
-      </c>
-      <c r="C6" s="54">
-        <v>0</v>
-      </c>
-      <c r="D6" s="55">
+      <c r="B6" s="50">
+        <v>0</v>
+      </c>
+      <c r="C6" s="51">
+        <v>0</v>
+      </c>
+      <c r="D6" s="52">
         <f t="shared" ref="D6:D8" si="4">(B6-C6)</f>
         <v>0</v>
       </c>
-      <c r="E6" s="45"/>
-      <c r="F6" s="53">
+      <c r="E6" s="42"/>
+      <c r="F6" s="50">
         <f>(Gantt!$B20)*100</f>
         <v>0</v>
       </c>
-      <c r="G6" s="54">
+      <c r="G6" s="51">
         <f>(Gantt!$C20)*100</f>
         <v>0</v>
       </c>
-      <c r="H6" s="55">
+      <c r="H6" s="52">
         <f t="shared" ref="H6:H8" si="5">(F6-G6)</f>
         <v>0</v>
       </c>
-      <c r="I6" s="49"/>
-      <c r="J6" s="53">
-        <v>0</v>
-      </c>
-      <c r="K6" s="54">
+      <c r="I6" s="46"/>
+      <c r="J6" s="50">
+        <v>0</v>
+      </c>
+      <c r="K6" s="51">
         <f>Meetings!B5*100</f>
         <v>150</v>
       </c>
-      <c r="L6" s="55">
+      <c r="L6" s="52">
         <f t="shared" ref="L6:L8" si="6">(J6-K6)</f>
         <v>-150</v>
       </c>
-      <c r="M6" s="49"/>
-      <c r="N6" s="53">
-        <v>0</v>
-      </c>
-      <c r="O6" s="54">
-        <v>0</v>
-      </c>
-      <c r="P6" s="55">
+      <c r="M6" s="46"/>
+      <c r="N6" s="50">
+        <v>0</v>
+      </c>
+      <c r="O6" s="51">
+        <v>0</v>
+      </c>
+      <c r="P6" s="52">
         <f t="shared" ref="P6:P8" si="7">(N6-O6)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="53">
-        <v>0</v>
-      </c>
-      <c r="C7" s="54">
-        <v>0</v>
-      </c>
-      <c r="D7" s="55">
+      <c r="B7" s="50">
+        <v>0</v>
+      </c>
+      <c r="C7" s="51">
+        <v>0</v>
+      </c>
+      <c r="D7" s="52">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E7" s="45"/>
-      <c r="F7" s="53">
+      <c r="E7" s="42"/>
+      <c r="F7" s="50">
         <f>(Gantt!$B28)*100</f>
         <v>0</v>
       </c>
-      <c r="G7" s="54">
+      <c r="G7" s="51">
         <f>(Gantt!$C28)*100</f>
         <v>0</v>
       </c>
-      <c r="H7" s="55">
+      <c r="H7" s="52">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I7" s="49"/>
-      <c r="J7" s="53">
-        <v>0</v>
-      </c>
-      <c r="K7" s="54">
+      <c r="I7" s="46"/>
+      <c r="J7" s="50">
+        <v>0</v>
+      </c>
+      <c r="K7" s="51">
         <f>Meetings!B6*100</f>
         <v>150</v>
       </c>
-      <c r="L7" s="55">
+      <c r="L7" s="52">
         <f t="shared" si="6"/>
         <v>-150</v>
       </c>
-      <c r="M7" s="49"/>
-      <c r="N7" s="53">
-        <v>0</v>
-      </c>
-      <c r="O7" s="54">
-        <v>0</v>
-      </c>
-      <c r="P7" s="55">
+      <c r="M7" s="46"/>
+      <c r="N7" s="50">
+        <v>0</v>
+      </c>
+      <c r="O7" s="51">
+        <v>0</v>
+      </c>
+      <c r="P7" s="52">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="16" thickBot="1">
+    <row r="8" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="56">
-        <v>0</v>
-      </c>
-      <c r="C8" s="57">
-        <v>0</v>
-      </c>
-      <c r="D8" s="58">
+      <c r="B8" s="53">
+        <v>0</v>
+      </c>
+      <c r="C8" s="54">
+        <v>0</v>
+      </c>
+      <c r="D8" s="55">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E8" s="45"/>
-      <c r="F8" s="53">
+      <c r="E8" s="42"/>
+      <c r="F8" s="50">
         <f>(Gantt!$B36)*100</f>
         <v>100</v>
       </c>
-      <c r="G8" s="54">
+      <c r="G8" s="51">
         <f>(Gantt!$C36)*100</f>
         <v>75</v>
       </c>
-      <c r="H8" s="55">
+      <c r="H8" s="52">
         <f t="shared" si="5"/>
         <v>25</v>
       </c>
-      <c r="I8" s="49"/>
-      <c r="J8" s="53">
-        <v>0</v>
-      </c>
-      <c r="K8" s="54">
+      <c r="I8" s="46"/>
+      <c r="J8" s="50">
+        <v>0</v>
+      </c>
+      <c r="K8" s="51">
         <f>Meetings!B7*100</f>
         <v>150</v>
       </c>
-      <c r="L8" s="55">
+      <c r="L8" s="52">
         <f t="shared" si="6"/>
         <v>-150</v>
       </c>
-      <c r="M8" s="49"/>
-      <c r="N8" s="56">
-        <v>0</v>
-      </c>
-      <c r="O8" s="57">
-        <v>0</v>
-      </c>
-      <c r="P8" s="58">
+      <c r="M8" s="46"/>
+      <c r="N8" s="53">
+        <v>0</v>
+      </c>
+      <c r="O8" s="54">
+        <v>0</v>
+      </c>
+      <c r="P8" s="55">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="16" thickBot="1">
+    <row r="9" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="59">
+      <c r="B9" s="56">
         <f>SUM(B3:B8)</f>
         <v>0</v>
       </c>
-      <c r="C9" s="60">
+      <c r="C9" s="57">
         <f>SUM(C3:C8)</f>
         <v>0</v>
       </c>
-      <c r="D9" s="61">
+      <c r="D9" s="58">
         <f>SUM(D3:D8)</f>
         <v>0</v>
       </c>
-      <c r="E9" s="45"/>
-      <c r="F9" s="62">
+      <c r="E9" s="42"/>
+      <c r="F9" s="59">
         <f>SUM(F3:F8)</f>
         <v>100</v>
       </c>
-      <c r="G9" s="63">
+      <c r="G9" s="60">
         <f>SUM(G3:G8)</f>
         <v>75</v>
       </c>
-      <c r="H9" s="64">
+      <c r="H9" s="61">
         <f>SUM(H3:H8)</f>
         <v>25</v>
       </c>
-      <c r="I9" s="49"/>
-      <c r="J9" s="62">
+      <c r="I9" s="46"/>
+      <c r="J9" s="59">
         <f>SUM(J3:J8)</f>
         <v>0</v>
       </c>
-      <c r="K9" s="63">
+      <c r="K9" s="60">
         <f>SUM(K3:K8)</f>
         <v>750</v>
       </c>
-      <c r="L9" s="64">
+      <c r="L9" s="61">
         <f>SUM(L3:L8)</f>
         <v>-750</v>
       </c>
-      <c r="M9" s="49"/>
-      <c r="N9" s="59">
+      <c r="M9" s="46"/>
+      <c r="N9" s="56">
         <f>SUM(N3:N8)</f>
         <v>0</v>
       </c>
-      <c r="O9" s="60">
+      <c r="O9" s="57">
         <f>SUM(O3:O8)</f>
         <v>0</v>
       </c>
-      <c r="P9" s="61">
+      <c r="P9" s="58">
         <f>SUM(P3:P8)</f>
         <v>0</v>
       </c>
@@ -1314,14 +1322,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
@@ -1329,7 +1337,7 @@
     <col min="6" max="6" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>38</v>
       </c>
@@ -1352,7 +1360,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>30</v>
       </c>
@@ -1360,7 +1368,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1394,7 +1402,7 @@
       <c r="Z3" s="5"/>
       <c r="AA3" s="5"/>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1428,7 +1436,7 @@
       <c r="Z4" s="5"/>
       <c r="AA4" s="5"/>
     </row>
-    <row r="5" spans="1:27">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1462,7 +1470,7 @@
       <c r="Z5" s="5"/>
       <c r="AA5" s="5"/>
     </row>
-    <row r="6" spans="1:27">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1477,7 +1485,7 @@
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="40"/>
+      <c r="J6" s="37"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
@@ -1496,7 +1504,7 @@
       <c r="Z6" s="5"/>
       <c r="AA6" s="5"/>
     </row>
-    <row r="7" spans="1:27">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1530,7 +1538,7 @@
       <c r="Z7" s="5"/>
       <c r="AA7" s="5"/>
     </row>
-    <row r="8" spans="1:27">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1564,7 +1572,7 @@
       <c r="Z8" s="5"/>
       <c r="AA8" s="5"/>
     </row>
-    <row r="9" spans="1:27">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1598,7 +1606,7 @@
       <c r="Z9" s="5"/>
       <c r="AA9" s="5"/>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1634,7 +1642,7 @@
       <c r="Z10" s="5"/>
       <c r="AA10" s="5"/>
     </row>
-    <row r="11" spans="1:27">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>31</v>
       </c>
@@ -1665,7 +1673,7 @@
       <c r="Z11" s="5"/>
       <c r="AA11" s="5"/>
     </row>
-    <row r="12" spans="1:27">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1699,7 +1707,7 @@
       <c r="Z12" s="5"/>
       <c r="AA12" s="5"/>
     </row>
-    <row r="13" spans="1:27">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1733,7 +1741,7 @@
       <c r="Z13" s="5"/>
       <c r="AA13" s="5"/>
     </row>
-    <row r="14" spans="1:27">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1767,7 +1775,7 @@
       <c r="Z14" s="5"/>
       <c r="AA14" s="5"/>
     </row>
-    <row r="15" spans="1:27">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1801,7 +1809,7 @@
       <c r="Z15" s="5"/>
       <c r="AA15" s="5"/>
     </row>
-    <row r="16" spans="1:27">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1835,7 +1843,7 @@
       <c r="Z16" s="5"/>
       <c r="AA16" s="5"/>
     </row>
-    <row r="17" spans="1:27">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1869,7 +1877,7 @@
       <c r="Z17" s="5"/>
       <c r="AA17" s="5"/>
     </row>
-    <row r="18" spans="1:27">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1903,7 +1911,7 @@
       <c r="Z18" s="5"/>
       <c r="AA18" s="5"/>
     </row>
-    <row r="19" spans="1:27">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1937,7 +1945,7 @@
       <c r="Z19" s="5"/>
       <c r="AA19" s="5"/>
     </row>
-    <row r="20" spans="1:27">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -1973,7 +1981,7 @@
       <c r="Z20" s="5"/>
       <c r="AA20" s="5"/>
     </row>
-    <row r="21" spans="1:27">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>32</v>
       </c>
@@ -2004,7 +2012,7 @@
       <c r="Z21" s="5"/>
       <c r="AA21" s="5"/>
     </row>
-    <row r="22" spans="1:27">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -2014,7 +2022,7 @@
       <c r="C22">
         <v>0</v>
       </c>
-      <c r="E22" s="40"/>
+      <c r="E22" s="37"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
@@ -2038,7 +2046,7 @@
       <c r="Z22" s="5"/>
       <c r="AA22" s="5"/>
     </row>
-    <row r="23" spans="1:27">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -2072,7 +2080,7 @@
       <c r="Z23" s="5"/>
       <c r="AA23" s="5"/>
     </row>
-    <row r="24" spans="1:27">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -2106,7 +2114,7 @@
       <c r="Z24" s="5"/>
       <c r="AA24" s="5"/>
     </row>
-    <row r="25" spans="1:27">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -2140,7 +2148,7 @@
       <c r="Z25" s="5"/>
       <c r="AA25" s="5"/>
     </row>
-    <row r="26" spans="1:27">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -2174,7 +2182,7 @@
       <c r="Z26" s="5"/>
       <c r="AA26" s="5"/>
     </row>
-    <row r="27" spans="1:27">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -2203,13 +2211,13 @@
       <c r="U27" s="5"/>
       <c r="V27" s="5"/>
       <c r="W27" s="5"/>
-      <c r="X27" s="41"/>
+      <c r="X27" s="38"/>
       <c r="Y27" s="5"/>
       <c r="Z27" s="5"/>
       <c r="AA27" s="5"/>
     </row>
-    <row r="28" spans="1:27">
-      <c r="A28" s="39" t="s">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A28" s="36" t="s">
         <v>29</v>
       </c>
       <c r="B28">
@@ -2244,7 +2252,7 @@
       <c r="Z28" s="5"/>
       <c r="AA28" s="5"/>
     </row>
-    <row r="29" spans="1:27">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>33</v>
       </c>
@@ -2275,7 +2283,7 @@
       <c r="Z29" s="5"/>
       <c r="AA29" s="5"/>
     </row>
-    <row r="30" spans="1:27">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -2309,7 +2317,7 @@
       <c r="Z30" s="5"/>
       <c r="AA30" s="5"/>
     </row>
-    <row r="31" spans="1:27">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>20</v>
       </c>
@@ -2343,7 +2351,7 @@
       <c r="Z31" s="5"/>
       <c r="AA31" s="5"/>
     </row>
-    <row r="32" spans="1:27">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>20</v>
       </c>
@@ -2377,7 +2385,7 @@
       <c r="Z32" s="5"/>
       <c r="AA32" s="5"/>
     </row>
-    <row r="33" spans="1:27">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>20</v>
       </c>
@@ -2411,7 +2419,7 @@
       <c r="Z33" s="5"/>
       <c r="AA33" s="5"/>
     </row>
-    <row r="34" spans="1:27">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -2445,7 +2453,7 @@
       <c r="Z34" s="5"/>
       <c r="AA34" s="5"/>
     </row>
-    <row r="35" spans="1:27">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>20</v>
       </c>
@@ -2479,8 +2487,8 @@
       <c r="Z35" s="5"/>
       <c r="AA35" s="5"/>
     </row>
-    <row r="36" spans="1:27">
-      <c r="A36" s="39" t="s">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A36" s="36" t="s">
         <v>29</v>
       </c>
       <c r="B36">
@@ -2515,7 +2523,7 @@
       <c r="Z36" s="5"/>
       <c r="AA36" s="5"/>
     </row>
-    <row r="37" spans="1:27">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>34</v>
       </c>
@@ -2546,7 +2554,7 @@
       <c r="Z37" s="5"/>
       <c r="AA37" s="5"/>
     </row>
-    <row r="38" spans="1:27">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>20</v>
       </c>
@@ -2580,7 +2588,7 @@
       <c r="Z38" s="5"/>
       <c r="AA38" s="5"/>
     </row>
-    <row r="39" spans="1:27">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>20</v>
       </c>
@@ -2614,7 +2622,7 @@
       <c r="Z39" s="5"/>
       <c r="AA39" s="5"/>
     </row>
-    <row r="40" spans="1:27">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>20</v>
       </c>
@@ -2648,7 +2656,7 @@
       <c r="Z40" s="5"/>
       <c r="AA40" s="5"/>
     </row>
-    <row r="41" spans="1:27">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>20</v>
       </c>
@@ -2663,7 +2671,7 @@
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
-      <c r="J41" s="40"/>
+      <c r="J41" s="37"/>
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
       <c r="M41" s="5"/>
@@ -2682,7 +2690,7 @@
       <c r="Z41" s="5"/>
       <c r="AA41" s="5"/>
     </row>
-    <row r="42" spans="1:27">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>20</v>
       </c>
@@ -2716,7 +2724,7 @@
       <c r="Z42" s="5"/>
       <c r="AA42" s="5"/>
     </row>
-    <row r="43" spans="1:27">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>20</v>
       </c>
@@ -2750,7 +2758,7 @@
       <c r="Z43" s="5"/>
       <c r="AA43" s="5"/>
     </row>
-    <row r="44" spans="1:27">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>20</v>
       </c>
@@ -2784,7 +2792,7 @@
       <c r="Z44" s="5"/>
       <c r="AA44" s="5"/>
     </row>
-    <row r="45" spans="1:27">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>29</v>
       </c>
@@ -2820,7 +2828,7 @@
       <c r="Z45" s="5"/>
       <c r="AA45" s="5"/>
     </row>
-    <row r="46" spans="1:27">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>35</v>
       </c>
@@ -2851,7 +2859,7 @@
       <c r="Z46" s="5"/>
       <c r="AA46" s="5"/>
     </row>
-    <row r="47" spans="1:27">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>20</v>
       </c>
@@ -2885,7 +2893,7 @@
       <c r="Z47" s="5"/>
       <c r="AA47" s="5"/>
     </row>
-    <row r="48" spans="1:27">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>20</v>
       </c>
@@ -2919,7 +2927,7 @@
       <c r="Z48" s="5"/>
       <c r="AA48" s="5"/>
     </row>
-    <row r="49" spans="1:27">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>20</v>
       </c>
@@ -2953,7 +2961,7 @@
       <c r="Z49" s="5"/>
       <c r="AA49" s="5"/>
     </row>
-    <row r="50" spans="1:27">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>20</v>
       </c>
@@ -2987,7 +2995,7 @@
       <c r="Z50" s="5"/>
       <c r="AA50" s="5"/>
     </row>
-    <row r="51" spans="1:27">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>20</v>
       </c>
@@ -3021,7 +3029,7 @@
       <c r="Z51" s="5"/>
       <c r="AA51" s="5"/>
     </row>
-    <row r="52" spans="1:27">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>20</v>
       </c>
@@ -3055,7 +3063,7 @@
       <c r="Z52" s="5"/>
       <c r="AA52" s="5"/>
     </row>
-    <row r="53" spans="1:27">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>20</v>
       </c>
@@ -3089,7 +3097,7 @@
       <c r="Z53" s="5"/>
       <c r="AA53" s="5"/>
     </row>
-    <row r="54" spans="1:27">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>20</v>
       </c>
@@ -3123,7 +3131,7 @@
       <c r="Z54" s="5"/>
       <c r="AA54" s="5"/>
     </row>
-    <row r="55" spans="1:27">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>29</v>
       </c>
@@ -3159,7 +3167,7 @@
       <c r="Z55" s="5"/>
       <c r="AA55" s="5"/>
     </row>
-    <row r="56" spans="1:27">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>0</v>
       </c>
@@ -3195,7 +3203,7 @@
       <c r="Z56" s="5"/>
       <c r="AA56" s="5"/>
     </row>
-    <row r="57" spans="1:27">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>1</v>
       </c>
@@ -3214,317 +3222,317 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5" style="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="31"/>
-    <col min="3" max="3" width="7.33203125" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.1640625" style="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5" style="31" customWidth="1"/>
-    <col min="6" max="6" width="10.5" style="31" customWidth="1"/>
-    <col min="7" max="9" width="8.83203125" style="31"/>
-    <col min="10" max="10" width="6.6640625" style="31" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9" style="31" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.1640625" style="31" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="31"/>
+    <col min="1" max="1" width="15.5" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="28"/>
+    <col min="3" max="3" width="7.33203125" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" style="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5" style="28" customWidth="1"/>
+    <col min="6" max="6" width="10.5" style="28" customWidth="1"/>
+    <col min="7" max="9" width="8.83203125" style="28"/>
+    <col min="10" max="10" width="6.6640625" style="28" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" style="28" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1640625" style="28" customWidth="1"/>
+    <col min="13" max="16384" width="8.83203125" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="65" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="37" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="62.25" customHeight="1">
-      <c r="B2" s="32" t="s">
+      <c r="D1" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="G2" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="H2" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="33" t="s">
+      <c r="I2" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="33" t="s">
+      <c r="J2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="33" t="s">
+      <c r="K2" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="33" t="s">
+      <c r="L2" s="30" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
-      <c r="B3" s="32" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B3" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="37">
+      <c r="C3" s="34">
         <v>1.5</v>
       </c>
-      <c r="D3" s="37">
-        <v>0</v>
-      </c>
-      <c r="E3" s="37">
-        <v>0</v>
-      </c>
-      <c r="F3" s="37">
-        <v>0</v>
-      </c>
-      <c r="G3" s="37">
-        <v>0</v>
-      </c>
-      <c r="H3" s="37">
-        <v>0</v>
-      </c>
-      <c r="I3" s="37">
-        <v>0</v>
-      </c>
-      <c r="J3" s="37">
-        <v>0</v>
-      </c>
-      <c r="K3" s="37">
-        <v>0</v>
-      </c>
-      <c r="L3" s="37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="32" t="s">
+      <c r="D3" s="34">
+        <v>0</v>
+      </c>
+      <c r="E3" s="34">
+        <v>0</v>
+      </c>
+      <c r="F3" s="34">
+        <v>0</v>
+      </c>
+      <c r="G3" s="34">
+        <v>0</v>
+      </c>
+      <c r="H3" s="34">
+        <v>0</v>
+      </c>
+      <c r="I3" s="34">
+        <v>0</v>
+      </c>
+      <c r="J3" s="34">
+        <v>0</v>
+      </c>
+      <c r="K3" s="34">
+        <v>0</v>
+      </c>
+      <c r="L3" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="32">
-        <f>SUMIF(C4:L4,A$1,C$3:Z$3)</f>
+      <c r="B4" s="29">
+        <f t="shared" ref="B4:B9" si="0">SUMIF(C4:L4,A$1,C$3:Z$3)</f>
         <v>1.5</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="32" t="s">
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="32">
-        <f>SUMIF(C5:L5,A$1,C$3:Z$3)</f>
+      <c r="B5" s="29">
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="32" t="s">
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="32">
-        <f>SUMIF(C6:L6,A$1,C$3:Z$3)</f>
+      <c r="B6" s="29">
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="32" t="s">
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="32">
-        <f>SUMIF(C7:L7,A$1,C$3:Z$3)</f>
+      <c r="B7" s="29">
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="32" t="s">
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="32">
-        <f>SUMIF(C8:L8,A$1,C$3:Z$3)</f>
+      <c r="B8" s="29">
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34"/>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="32" t="s">
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="32">
-        <f>SUMIF(C9:L9,A$1,C$3:Z$3)</f>
+      <c r="B9" s="29">
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="34"/>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="32" t="s">
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="35">
+      <c r="B10" s="32">
         <f>SUM(B4:B9)</f>
         <v>9</v>
       </c>
-      <c r="C10" s="38">
-        <f>COUNTIF(C4:C9,"*ü*") * C3</f>
+      <c r="C10" s="35">
+        <f t="shared" ref="C10:L10" si="1">COUNTIF(C4:C9,"*ü*") * C3</f>
         <v>9</v>
       </c>
-      <c r="D10" s="38">
-        <f>COUNTIF(D4:D9,"*ü*") * D3</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="38">
-        <f>COUNTIF(E4:E9,"*ü*") * E3</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="38">
-        <f>COUNTIF(F4:F9,"*ü*") * F3</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="38">
-        <f>COUNTIF(G4:G9,"*ü*") * G3</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="38">
-        <f>COUNTIF(H4:H9,"*ü*") * H3</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="38">
-        <f>COUNTIF(I4:I9,"*ü*") * I3</f>
-        <v>0</v>
-      </c>
-      <c r="J10" s="38">
-        <f>COUNTIF(J4:J9,"*ü*") * J3</f>
-        <v>0</v>
-      </c>
-      <c r="K10" s="38">
-        <f>COUNTIF(K4:K9,"*ü*") * K3</f>
-        <v>0</v>
-      </c>
-      <c r="L10" s="38">
-        <f>COUNTIF(L4:L9,"*ü*") * L3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="36"/>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="34"/>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="34"/>
+      <c r="D10" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E10" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K10" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L10" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="33"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="31"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3533,14 +3541,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.6640625" customWidth="1"/>
@@ -3549,7 +3557,7 @@
     <col min="5" max="19" width="3.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="13"/>
       <c r="B1" s="14" t="s">
         <v>36</v>
@@ -3606,7 +3614,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>30</v>
       </c>
@@ -3631,7 +3639,7 @@
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="27"/>
       <c r="B3" s="17" t="s">
         <v>20</v>
@@ -3654,7 +3662,7 @@
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="20"/>
       <c r="B4" s="17" t="s">
         <v>20</v>
@@ -3670,14 +3678,14 @@
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="66"/>
+      <c r="J4" s="63"/>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="20"/>
       <c r="B5" s="17" t="s">
         <v>17</v>
@@ -3702,7 +3710,7 @@
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>31</v>
       </c>
@@ -3727,7 +3735,7 @@
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="27"/>
       <c r="B7" s="17" t="s">
         <v>20</v>
@@ -3750,7 +3758,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="20"/>
       <c r="B8" s="17" t="s">
         <v>20</v>
@@ -3766,14 +3774,14 @@
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
-      <c r="J8" s="66"/>
+      <c r="J8" s="63"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="20"/>
       <c r="B9" s="17" t="s">
         <v>17</v>
@@ -3798,7 +3806,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>32</v>
       </c>
@@ -3823,7 +3831,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="27"/>
       <c r="B11" s="17" t="s">
         <v>20</v>
@@ -3846,7 +3854,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="20"/>
       <c r="B12" s="17" t="s">
         <v>20</v>
@@ -3863,13 +3871,13 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="66"/>
+      <c r="K12" s="63"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="20"/>
       <c r="B13" s="17" t="s">
         <v>20</v>
@@ -3892,7 +3900,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="20"/>
       <c r="B14" s="17" t="s">
         <v>20</v>
@@ -3915,7 +3923,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="20"/>
       <c r="B15" s="22" t="s">
         <v>17</v>
@@ -3940,7 +3948,7 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
         <v>33</v>
       </c>
@@ -3965,7 +3973,7 @@
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="27"/>
       <c r="B17" s="17" t="s">
         <v>20</v>
@@ -3988,7 +3996,7 @@
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="20"/>
       <c r="B18" s="17" t="s">
         <v>20</v>
@@ -4004,14 +4012,14 @@
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
-      <c r="J18" s="66"/>
+      <c r="J18" s="63"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="20"/>
       <c r="B19" s="17" t="s">
         <v>17</v>
@@ -4036,18 +4044,18 @@
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
         <v>34</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C20" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -4061,7 +4069,7 @@
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="27"/>
       <c r="B21" s="17" t="s">
         <v>20</v>
@@ -4084,7 +4092,7 @@
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="20"/>
       <c r="B22" s="17" t="s">
         <v>20</v>
@@ -4101,13 +4109,13 @@
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
-      <c r="K22" s="66"/>
+      <c r="K22" s="63"/>
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="20"/>
       <c r="B23" s="17" t="s">
         <v>20</v>
@@ -4130,7 +4138,7 @@
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="20"/>
       <c r="B24" s="17" t="s">
         <v>20</v>
@@ -4153,18 +4161,18 @@
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="20"/>
       <c r="B25" s="22" t="s">
         <v>17</v>
       </c>
       <c r="C25" s="17">
         <f>SUM(C20:C24)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" s="21">
         <f>SUM(D20:D24)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -4178,7 +4186,7 @@
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">
         <v>35</v>
       </c>
@@ -4203,7 +4211,7 @@
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="27"/>
       <c r="B27" s="17" t="s">
         <v>20</v>
@@ -4226,7 +4234,7 @@
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="20"/>
       <c r="B28" s="17" t="s">
         <v>20</v>
@@ -4242,14 +4250,14 @@
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
-      <c r="J28" s="66"/>
+      <c r="J28" s="63"/>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
       <c r="O28" s="5"/>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="20"/>
       <c r="B29" s="22" t="s">
         <v>39</v>
@@ -4274,7 +4282,7 @@
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
     </row>
-    <row r="30" spans="1:15" ht="16" thickBot="1">
+    <row r="30" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="23"/>
       <c r="B30" s="24" t="s">
         <v>29</v>
@@ -4299,7 +4307,7 @@
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B31" s="12"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Master Gantt Chart
</commit_message>
<xml_diff>
--- a/Documents/Master Gantt.xlsx
+++ b/Documents/Master Gantt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BenjaminHallman/Documents/College/Classes/Computer Science/383/Projects/Dream Team/Maze Runner/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA1624C-D91E-8445-98E9-EF2514D2704B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777CAAFD-D313-8C40-B424-EED794D1F746}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Management Summary" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="42">
   <si>
     <t>Total</t>
   </si>
@@ -165,6 +165,18 @@
   </si>
   <si>
     <t>TDB</t>
+  </si>
+  <si>
+    <t>Logo Design</t>
+  </si>
+  <si>
+    <t>Setup Master Gantt</t>
+  </si>
+  <si>
+    <t>Coding Standards</t>
+  </si>
+  <si>
+    <t>GitHub and Discord Setup</t>
   </si>
 </sst>
 </file>
@@ -894,7 +906,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
@@ -988,29 +1000,29 @@
         <v>7</v>
       </c>
       <c r="B3" s="11">
-        <f>(SUM(F3,J3,N3))</f>
-        <v>500</v>
+        <f t="shared" ref="B3:C8" si="0">(SUM(F3,J3,N3))</f>
+        <v>1500</v>
       </c>
       <c r="C3" s="12">
-        <f>(SUM(G3,K3,O3))</f>
-        <v>150</v>
+        <f t="shared" si="0"/>
+        <v>200</v>
       </c>
       <c r="D3" s="13">
-        <f t="shared" ref="D3:D8" si="0">(B3-C3)</f>
-        <v>350</v>
+        <f t="shared" ref="D3:D8" si="1">(B3-C3)</f>
+        <v>1300</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="14">
         <f>(Gantt!$B13)*100</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G3" s="15">
         <f>(Gantt!$C13)*100</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="H3" s="16">
-        <f t="shared" ref="H3:H8" si="1">(F3-G3)</f>
-        <v>0</v>
+        <f t="shared" ref="H3:H8" si="2">(F3-G3)</f>
+        <v>50</v>
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="11">
@@ -1021,21 +1033,21 @@
         <v>150</v>
       </c>
       <c r="L3" s="13">
-        <f t="shared" ref="L3:L8" si="2">(J3-K3)</f>
+        <f t="shared" ref="L3:L8" si="3">(J3-K3)</f>
         <v>350</v>
       </c>
       <c r="M3" s="9"/>
       <c r="N3" s="11">
         <f>SA!C5*100</f>
-        <v>0</v>
+        <v>900</v>
       </c>
       <c r="O3" s="12">
         <f>SA!D5*100</f>
         <v>0</v>
       </c>
       <c r="P3" s="13">
-        <f t="shared" ref="P3:P8" si="3">(N3-O3)</f>
-        <v>0</v>
+        <f t="shared" ref="P3:P8" si="4">(N3-O3)</f>
+        <v>900</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -1043,16 +1055,16 @@
         <v>8</v>
       </c>
       <c r="B4" s="14">
-        <f>(SUM(F4,J4,N4))</f>
-        <v>500</v>
+        <f t="shared" si="0"/>
+        <v>1400</v>
       </c>
       <c r="C4" s="15">
-        <f>(SUM(G4,K4,O4))</f>
+        <f t="shared" si="0"/>
         <v>150</v>
       </c>
       <c r="D4" s="16">
-        <f t="shared" si="0"/>
-        <v>350</v>
+        <f t="shared" si="1"/>
+        <v>1250</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="14">
@@ -1064,7 +1076,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I4" s="9"/>
@@ -1076,21 +1088,21 @@
         <v>150</v>
       </c>
       <c r="L4" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>350</v>
       </c>
       <c r="M4" s="9"/>
       <c r="N4" s="14">
         <f>SA!C9*100</f>
-        <v>0</v>
+        <v>900</v>
       </c>
       <c r="O4" s="15">
         <f>SA!D9*100</f>
         <v>0</v>
       </c>
       <c r="P4" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>900</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1098,16 +1110,16 @@
         <v>9</v>
       </c>
       <c r="B5" s="14">
-        <f>(SUM(F5,J5,N5))</f>
-        <v>500</v>
+        <f t="shared" si="0"/>
+        <v>1400</v>
       </c>
       <c r="C5" s="15">
-        <f>(SUM(G5,K5,O5))</f>
-        <v>150</v>
+        <f t="shared" si="0"/>
+        <v>200</v>
       </c>
       <c r="D5" s="16">
-        <f t="shared" si="0"/>
-        <v>350</v>
+        <f t="shared" si="1"/>
+        <v>1200</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="14">
@@ -1119,7 +1131,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I5" s="9"/>
@@ -1128,24 +1140,24 @@
       </c>
       <c r="K5" s="15">
         <f>Meetings!B6*100</f>
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="L5" s="16">
-        <f t="shared" si="2"/>
-        <v>350</v>
+        <f t="shared" si="3"/>
+        <v>300</v>
       </c>
       <c r="M5" s="9"/>
       <c r="N5" s="14">
         <f>SA!C13*100</f>
-        <v>0</v>
+        <v>900</v>
       </c>
       <c r="O5" s="15">
         <f>SA!D13*100</f>
         <v>0</v>
       </c>
       <c r="P5" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>900</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1153,16 +1165,16 @@
         <v>10</v>
       </c>
       <c r="B6" s="14">
-        <f>(SUM(F6,J6,N6))</f>
-        <v>500</v>
+        <f t="shared" si="0"/>
+        <v>1400</v>
       </c>
       <c r="C6" s="15">
-        <f>(SUM(G6,K6,O6))</f>
-        <v>150</v>
+        <f t="shared" si="0"/>
+        <v>200</v>
       </c>
       <c r="D6" s="16">
-        <f t="shared" si="0"/>
-        <v>350</v>
+        <f t="shared" si="1"/>
+        <v>1200</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="14">
@@ -1174,7 +1186,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I6" s="9"/>
@@ -1183,24 +1195,24 @@
       </c>
       <c r="K6" s="15">
         <f>Meetings!B7*100</f>
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="L6" s="16">
-        <f t="shared" si="2"/>
-        <v>350</v>
+        <f t="shared" si="3"/>
+        <v>300</v>
       </c>
       <c r="M6" s="9"/>
       <c r="N6" s="14">
         <f>SA!C17*100</f>
-        <v>0</v>
+        <v>900</v>
       </c>
       <c r="O6" s="15">
         <f>SA!D17*100</f>
         <v>0</v>
       </c>
       <c r="P6" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>900</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1208,29 +1220,29 @@
         <v>11</v>
       </c>
       <c r="B7" s="14">
-        <f>(SUM(F7,J7,N7))</f>
-        <v>500</v>
+        <f t="shared" si="0"/>
+        <v>1500</v>
       </c>
       <c r="C7" s="15">
-        <f>(SUM(G7,K7,O7))</f>
-        <v>150</v>
+        <f t="shared" si="0"/>
+        <v>400</v>
       </c>
       <c r="D7" s="16">
-        <f t="shared" si="0"/>
-        <v>350</v>
+        <f t="shared" si="1"/>
+        <v>1100</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="14">
         <f>(Gantt!$B61)*100</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G7" s="15">
         <f>(Gantt!$C61)*100</f>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="H7" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>-100</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="14">
@@ -1238,24 +1250,24 @@
       </c>
       <c r="K7" s="15">
         <f>Meetings!B8*100</f>
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="L7" s="16">
-        <f t="shared" si="2"/>
-        <v>350</v>
+        <f t="shared" si="3"/>
+        <v>300</v>
       </c>
       <c r="M7" s="9"/>
       <c r="N7" s="14">
         <f>SA!C21*100</f>
-        <v>0</v>
+        <v>900</v>
       </c>
       <c r="O7" s="15">
         <f>SA!D21*100</f>
         <v>0</v>
       </c>
       <c r="P7" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>900</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1263,29 +1275,29 @@
         <v>12</v>
       </c>
       <c r="B8" s="18">
-        <f>(SUM(F8,J8,N8))</f>
-        <v>500</v>
+        <f t="shared" si="0"/>
+        <v>1500</v>
       </c>
       <c r="C8" s="19">
-        <f>(SUM(G8,K8,O8))</f>
-        <v>150</v>
+        <f t="shared" si="0"/>
+        <v>220</v>
       </c>
       <c r="D8" s="20">
-        <f t="shared" si="0"/>
-        <v>350</v>
+        <f t="shared" si="1"/>
+        <v>1280</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="14">
         <f>(Gantt!$B73)*100</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G8" s="15">
         <f>(Gantt!$C73)*100</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H8" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>80</v>
       </c>
       <c r="I8" s="9"/>
       <c r="J8" s="14">
@@ -1293,24 +1305,24 @@
       </c>
       <c r="K8" s="15">
         <f>Meetings!B9*100</f>
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="L8" s="16">
-        <f t="shared" si="2"/>
-        <v>350</v>
+        <f t="shared" si="3"/>
+        <v>300</v>
       </c>
       <c r="M8" s="9"/>
       <c r="N8" s="18">
         <f>SA!C25*100</f>
-        <v>0</v>
+        <v>900</v>
       </c>
       <c r="O8" s="19">
         <f>SA!D25*100</f>
         <v>0</v>
       </c>
       <c r="P8" s="20">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>900</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1319,28 +1331,28 @@
       </c>
       <c r="B9" s="22">
         <f>SUM(B3:B8)</f>
-        <v>3000</v>
+        <v>8700</v>
       </c>
       <c r="C9" s="23">
         <f>SUM(C3:C8)</f>
-        <v>900</v>
+        <v>1370</v>
       </c>
       <c r="D9" s="24">
         <f>SUM(D3:D8)</f>
-        <v>2100</v>
+        <v>7330</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="25">
         <f>SUM(F3:F8)</f>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="G9" s="26">
         <f>SUM(G3:G8)</f>
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="H9" s="27">
         <f>SUM(H3:H8)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="25">
@@ -1349,16 +1361,16 @@
       </c>
       <c r="K9" s="26">
         <f>SUM(K3:K8)</f>
-        <v>900</v>
+        <v>1100</v>
       </c>
       <c r="L9" s="27">
         <f>SUM(L3:L8)</f>
-        <v>2100</v>
+        <v>1900</v>
       </c>
       <c r="M9" s="9"/>
       <c r="N9" s="22">
         <f>SUM(N3:N8)</f>
-        <v>0</v>
+        <v>5400</v>
       </c>
       <c r="O9" s="23">
         <f>SUM(O3:O8)</f>
@@ -1366,7 +1378,7 @@
       </c>
       <c r="P9" s="24">
         <f>SUM(P3:P8)</f>
-        <v>0</v>
+        <v>5400</v>
       </c>
     </row>
   </sheetData>
@@ -1385,8 +1397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1432,13 +1444,13 @@
     </row>
     <row r="3" spans="1:27">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E3" s="32"/>
       <c r="F3" s="32"/>
@@ -1707,11 +1719,11 @@
       </c>
       <c r="B13">
         <f>SUM(B3:B12)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <f>SUM(C3:C12)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E13" s="32"/>
       <c r="F13" s="32"/>
@@ -2126,7 +2138,7 @@
     </row>
     <row r="39" spans="1:27" s="32" customFormat="1">
       <c r="A39" s="32" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="B39" s="32">
         <v>0</v>
@@ -2304,13 +2316,13 @@
     </row>
     <row r="51" spans="1:27" s="32" customFormat="1">
       <c r="A51" s="32" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="B51" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C51" s="32">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:27" s="32" customFormat="1">
@@ -2419,11 +2431,11 @@
       </c>
       <c r="B61">
         <f>SUM(B51:B60)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C61">
         <f>SUM(C51:C60)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E61" s="32"/>
       <c r="F61" s="32"/>
@@ -2482,13 +2494,13 @@
     </row>
     <row r="63" spans="1:27" s="32" customFormat="1">
       <c r="A63" s="32" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="B63" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C63" s="32">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="64" spans="1:27" s="32" customFormat="1">
@@ -2597,11 +2609,11 @@
       </c>
       <c r="B73">
         <f>SUM(B63:B72)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C73">
         <f>SUM(C63:C72)</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E73" s="32"/>
       <c r="F73" s="32"/>
@@ -2633,11 +2645,11 @@
       </c>
       <c r="B74">
         <f>SUM(B13,B25,B37,B49,B61,B73)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C74">
         <f>SUM(C13,C25,C37,C49,C61,C73)</f>
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="E74" s="32"/>
       <c r="F74" s="32"/>
@@ -2669,11 +2681,11 @@
       </c>
       <c r="B75" s="36">
         <f>B74*100</f>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="C75" s="36">
         <f>C74*100</f>
-        <v>0</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -2687,7 +2699,7 @@
   <dimension ref="A1:AMK10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2786,7 +2798,7 @@
         <v>1.5</v>
       </c>
       <c r="D3" s="40">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E3" s="40">
         <v>0</v>
@@ -2859,12 +2871,14 @@
       </c>
       <c r="B6" s="39">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="C6" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="42"/>
+      <c r="D6" s="38" t="s">
+        <v>24</v>
+      </c>
       <c r="E6" s="42"/>
       <c r="F6" s="42"/>
       <c r="G6" s="42"/>
@@ -2880,12 +2894,14 @@
       </c>
       <c r="B7" s="39">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="C7" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="42"/>
+      <c r="D7" s="38" t="s">
+        <v>24</v>
+      </c>
       <c r="E7" s="42"/>
       <c r="F7" s="42"/>
       <c r="G7" s="42"/>
@@ -2901,12 +2917,14 @@
       </c>
       <c r="B8" s="39">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="C8" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="42"/>
+      <c r="D8" s="38" t="s">
+        <v>24</v>
+      </c>
       <c r="E8" s="42"/>
       <c r="F8" s="42"/>
       <c r="G8" s="42"/>
@@ -2922,12 +2940,14 @@
       </c>
       <c r="B9" s="39">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="C9" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="42"/>
+      <c r="D9" s="38" t="s">
+        <v>24</v>
+      </c>
       <c r="E9" s="42"/>
       <c r="F9" s="42"/>
       <c r="G9" s="42"/>
@@ -2943,7 +2963,7 @@
       </c>
       <c r="B10" s="39">
         <f>SUM(B4:B9)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C10" s="40">
         <f t="shared" ref="C10:L10" si="1">COUNTIF(C4:C9,"*ü*") * C3</f>
@@ -2951,7 +2971,7 @@
       </c>
       <c r="D10" s="40">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E10" s="40">
         <f t="shared" si="1"/>
@@ -2997,7 +3017,7 @@
   <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3075,7 +3095,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="47">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D2" s="48">
         <v>0</v>
@@ -3098,7 +3118,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="47">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D3" s="48">
         <v>0</v>
@@ -3121,7 +3141,7 @@
         <v>33</v>
       </c>
       <c r="C4" s="47">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D4" s="48">
         <v>0</v>
@@ -3135,7 +3155,7 @@
       </c>
       <c r="C5" s="46">
         <f>SUM(C2:C4)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D5" s="51">
         <f>SUM(D2:D4)</f>
@@ -3161,7 +3181,7 @@
         <v>31</v>
       </c>
       <c r="C6" s="47">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D6" s="48">
         <v>0</v>
@@ -3173,7 +3193,7 @@
         <v>32</v>
       </c>
       <c r="C7" s="47">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D7" s="48">
         <v>0</v>
@@ -3186,7 +3206,7 @@
         <v>33</v>
       </c>
       <c r="C8" s="47">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D8" s="48">
         <v>0</v>
@@ -3200,7 +3220,7 @@
       </c>
       <c r="C9" s="46">
         <f>SUM(C6:C8)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D9" s="51">
         <f>SUM(D6:D8)</f>
@@ -3226,7 +3246,7 @@
         <v>31</v>
       </c>
       <c r="C10" s="47">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D10" s="48">
         <v>0</v>
@@ -3238,7 +3258,7 @@
         <v>32</v>
       </c>
       <c r="C11" s="47">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D11" s="48">
         <v>0</v>
@@ -3251,7 +3271,7 @@
         <v>33</v>
       </c>
       <c r="C12" s="47">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D12" s="48">
         <v>0</v>
@@ -3265,7 +3285,7 @@
       </c>
       <c r="C13" s="46">
         <f>SUM(C10:C12)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D13" s="51">
         <f>SUM(D10:D12)</f>
@@ -3291,7 +3311,7 @@
         <v>31</v>
       </c>
       <c r="C14" s="47">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D14" s="48">
         <v>0</v>
@@ -3303,7 +3323,7 @@
         <v>32</v>
       </c>
       <c r="C15" s="47">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D15" s="48">
         <v>0</v>
@@ -3316,7 +3336,7 @@
         <v>33</v>
       </c>
       <c r="C16" s="47">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D16" s="48">
         <v>0</v>
@@ -3330,7 +3350,7 @@
       </c>
       <c r="C17" s="46">
         <f>SUM(C14:C16)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D17" s="51">
         <f>SUM(D14:D16)</f>
@@ -3356,7 +3376,7 @@
         <v>31</v>
       </c>
       <c r="C18" s="47">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D18" s="48">
         <v>0</v>
@@ -3368,7 +3388,7 @@
         <v>32</v>
       </c>
       <c r="C19" s="47">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D19" s="48">
         <v>0</v>
@@ -3381,7 +3401,7 @@
         <v>33</v>
       </c>
       <c r="C20" s="47">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D20" s="48">
         <v>0</v>
@@ -3395,7 +3415,7 @@
       </c>
       <c r="C21" s="46">
         <f>SUM(C18:C20)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D21" s="51">
         <f>SUM(D18:D20)</f>
@@ -3421,7 +3441,7 @@
         <v>31</v>
       </c>
       <c r="C22" s="47">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D22" s="48">
         <v>0</v>
@@ -3433,7 +3453,7 @@
         <v>32</v>
       </c>
       <c r="C23" s="47">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D23" s="48">
         <v>0</v>
@@ -3446,7 +3466,7 @@
         <v>33</v>
       </c>
       <c r="C24" s="47">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D24" s="48">
         <v>0</v>
@@ -3460,7 +3480,7 @@
       </c>
       <c r="C25" s="46">
         <f>SUM(C22:C24)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D25" s="51">
         <f>SUM(D22:D24)</f>
@@ -3485,7 +3505,7 @@
       </c>
       <c r="C26" s="55">
         <f>SUM(C5,C9,C13,C17,C21,C25)</f>
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="D26" s="56">
         <f>SUM(D5,D9,D13,D17,D21,D25)</f>

</xml_diff>

<commit_message>
Update Gantt Chart with Item Manager Tasks
</commit_message>
<xml_diff>
--- a/Documents/Master Gantt.xlsx
+++ b/Documents/Master Gantt.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27510"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cameron\Documents\GitHub\Maze_Runner\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Delaney/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B212808-61CE-4AA8-8F57-DA25EDCC0703}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="12820" windowHeight="15240" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Management Summary" sheetId="1" r:id="rId1"/>
@@ -18,8 +17,14 @@
     <sheet name="Meetings" sheetId="3" r:id="rId3"/>
     <sheet name="SA" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -34,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="72">
   <si>
     <t>Total</t>
   </si>
@@ -260,16 +265,25 @@
   <si>
     <t>Make stuff work together</t>
   </si>
+  <si>
+    <t>Function Definitions</t>
+  </si>
+  <si>
+    <t>User Documentation</t>
+  </si>
+  <si>
+    <t>Programming</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="\$#,##0.00_);[Red]&quot;($&quot;#,##0.00\)"/>
     <numFmt numFmtId="165" formatCode="\$#,##0.00;[Red]\$#,##0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -985,35 +999,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.453125" customWidth="1"/>
-    <col min="2" max="2" width="14.36328125" customWidth="1"/>
-    <col min="3" max="3" width="13.81640625" customWidth="1"/>
-    <col min="4" max="4" width="13.36328125" customWidth="1"/>
-    <col min="5" max="5" width="3.453125" customWidth="1"/>
-    <col min="6" max="6" width="15.36328125" customWidth="1"/>
-    <col min="7" max="7" width="12.36328125" customWidth="1"/>
-    <col min="8" max="8" width="14.453125" customWidth="1"/>
-    <col min="9" max="9" width="2.81640625" customWidth="1"/>
-    <col min="10" max="10" width="13.81640625" customWidth="1"/>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="3.5" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="8" max="8" width="14.5" customWidth="1"/>
+    <col min="9" max="9" width="2.83203125" customWidth="1"/>
+    <col min="10" max="10" width="13.83203125" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="12" max="12" width="14.1796875" customWidth="1"/>
-    <col min="13" max="13" width="5.453125" customWidth="1"/>
-    <col min="14" max="14" width="12.36328125" customWidth="1"/>
-    <col min="15" max="15" width="14.6328125" customWidth="1"/>
-    <col min="16" max="16" width="11.36328125" customWidth="1"/>
-    <col min="17" max="1025" width="8.81640625" customWidth="1"/>
+    <col min="12" max="12" width="14.1640625" customWidth="1"/>
+    <col min="13" max="13" width="5.5" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" customWidth="1"/>
+    <col min="15" max="15" width="14.6640625" customWidth="1"/>
+    <col min="16" max="16" width="11.33203125" customWidth="1"/>
+    <col min="17" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B1" s="57" t="s">
         <v>0</v>
       </c>
@@ -1036,7 +1050,7 @@
       <c r="O1" s="57"/>
       <c r="P1" s="57"/>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1077,7 +1091,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>41</v>
       </c>
@@ -1132,7 +1146,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>42</v>
       </c>
@@ -1187,7 +1201,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>43</v>
       </c>
@@ -1242,7 +1256,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>44</v>
       </c>
@@ -1297,13 +1311,13 @@
         <v>450</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>45</v>
       </c>
       <c r="B7" s="14">
         <f t="shared" si="0"/>
-        <v>2700</v>
+        <v>4000</v>
       </c>
       <c r="C7" s="15">
         <f t="shared" si="0"/>
@@ -1311,12 +1325,12 @@
       </c>
       <c r="D7" s="16">
         <f t="shared" si="1"/>
-        <v>1725</v>
+        <v>3025</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="14">
         <f>(Gantt!$B61)*100</f>
-        <v>100</v>
+        <v>1400</v>
       </c>
       <c r="G7" s="15">
         <f>(Gantt!$C61)*100</f>
@@ -1324,7 +1338,7 @@
       </c>
       <c r="H7" s="16">
         <f t="shared" si="2"/>
-        <v>-100</v>
+        <v>1200</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="14">
@@ -1352,7 +1366,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>46</v>
       </c>
@@ -1407,13 +1421,13 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="22">
         <f>SUM(B3:B8)</f>
-        <v>16000</v>
+        <v>17300</v>
       </c>
       <c r="C9" s="23">
         <f>SUM(C3:C8)</f>
@@ -1421,12 +1435,12 @@
       </c>
       <c r="D9" s="24">
         <f>SUM(D3:D8)</f>
-        <v>9630</v>
+        <v>10930</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="25">
         <f>SUM(F3:F8)</f>
-        <v>400</v>
+        <v>1700</v>
       </c>
       <c r="G9" s="26">
         <f>SUM(G3:G8)</f>
@@ -1434,7 +1448,7 @@
       </c>
       <c r="H9" s="27">
         <f>SUM(H3:H8)</f>
-        <v>30</v>
+        <v>1330</v>
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="25">
@@ -1476,24 +1490,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="17.453125" customWidth="1"/>
-    <col min="3" max="3" width="15.6328125" customWidth="1"/>
-    <col min="4" max="5" width="8.81640625" customWidth="1"/>
-    <col min="6" max="6" width="10.6328125" customWidth="1"/>
-    <col min="7" max="1025" width="8.81640625" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="5" width="8.83203125" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="7" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>8</v>
       </c>
@@ -1516,7 +1530,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
         <v>41</v>
       </c>
@@ -1524,7 +1538,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1558,7 +1572,7 @@
       <c r="Z3" s="32"/>
       <c r="AA3" s="32"/>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1592,7 +1606,7 @@
       <c r="Z4" s="32"/>
       <c r="AA4" s="32"/>
     </row>
-    <row r="5" spans="1:27">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1626,7 +1640,7 @@
       <c r="Z5" s="32"/>
       <c r="AA5" s="32"/>
     </row>
-    <row r="6" spans="1:27">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1660,7 +1674,7 @@
       <c r="Z6" s="32"/>
       <c r="AA6" s="32"/>
     </row>
-    <row r="7" spans="1:27">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1694,7 +1708,7 @@
       <c r="Z7" s="32"/>
       <c r="AA7" s="32"/>
     </row>
-    <row r="8" spans="1:27">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1728,7 +1742,7 @@
       <c r="Z8" s="32"/>
       <c r="AA8" s="32"/>
     </row>
-    <row r="9" spans="1:27">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1762,7 +1776,7 @@
       <c r="Z9" s="32"/>
       <c r="AA9" s="32"/>
     </row>
-    <row r="10" spans="1:27" s="32" customFormat="1">
+    <row r="10" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
         <v>15</v>
       </c>
@@ -1773,7 +1787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:27" s="32" customFormat="1">
+    <row r="11" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
         <v>15</v>
       </c>
@@ -1784,7 +1798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:27" s="32" customFormat="1">
+    <row r="12" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="32" t="s">
         <v>15</v>
       </c>
@@ -1795,7 +1809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:27">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1831,7 +1845,7 @@
       <c r="Z13" s="32"/>
       <c r="AA13" s="32"/>
     </row>
-    <row r="14" spans="1:27">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" s="34" t="s">
         <v>42</v>
       </c>
@@ -1862,7 +1876,7 @@
       <c r="Z14" s="32"/>
       <c r="AA14" s="32"/>
     </row>
-    <row r="15" spans="1:27" s="32" customFormat="1">
+    <row r="15" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="32" t="s">
         <v>64</v>
       </c>
@@ -1873,7 +1887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:27" s="32" customFormat="1">
+    <row r="16" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="32" t="s">
         <v>66</v>
       </c>
@@ -1884,7 +1898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:27" s="32" customFormat="1">
+    <row r="17" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="32" t="s">
         <v>67</v>
       </c>
@@ -1895,7 +1909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:27" s="32" customFormat="1">
+    <row r="18" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="32" t="s">
         <v>65</v>
       </c>
@@ -1907,7 +1921,7 @@
       </c>
       <c r="J18" s="33"/>
     </row>
-    <row r="19" spans="1:27" s="32" customFormat="1">
+    <row r="19" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="32" t="s">
         <v>68</v>
       </c>
@@ -1918,7 +1932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:27" s="32" customFormat="1">
+    <row r="20" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="32" t="s">
         <v>61</v>
       </c>
@@ -1929,7 +1943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:27" s="32" customFormat="1">
+    <row r="21" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
         <v>63</v>
       </c>
@@ -1940,7 +1954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:27" s="32" customFormat="1">
+    <row r="22" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
         <v>15</v>
       </c>
@@ -1951,7 +1965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:27" s="32" customFormat="1">
+    <row r="23" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="32" t="s">
         <v>15</v>
       </c>
@@ -1962,7 +1976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:27" s="32" customFormat="1">
+    <row r="24" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="32" t="s">
         <v>15</v>
       </c>
@@ -1973,7 +1987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:27">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -2009,7 +2023,7 @@
       <c r="Z25" s="32"/>
       <c r="AA25" s="32"/>
     </row>
-    <row r="26" spans="1:27">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A26" s="34" t="s">
         <v>43</v>
       </c>
@@ -2040,7 +2054,7 @@
       <c r="Z26" s="32"/>
       <c r="AA26" s="32"/>
     </row>
-    <row r="27" spans="1:27" s="32" customFormat="1">
+    <row r="27" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="32" t="s">
         <v>15</v>
       </c>
@@ -2051,7 +2065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:27" s="32" customFormat="1">
+    <row r="28" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="32" t="s">
         <v>15</v>
       </c>
@@ -2062,7 +2076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:27" s="32" customFormat="1">
+    <row r="29" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="32" t="s">
         <v>15</v>
       </c>
@@ -2073,7 +2087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:27" s="32" customFormat="1">
+    <row r="30" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="32" t="s">
         <v>15</v>
       </c>
@@ -2085,7 +2099,7 @@
       </c>
       <c r="J30" s="33"/>
     </row>
-    <row r="31" spans="1:27" s="32" customFormat="1">
+    <row r="31" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="32" t="s">
         <v>15</v>
       </c>
@@ -2096,7 +2110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:27" s="32" customFormat="1">
+    <row r="32" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="32" t="s">
         <v>15</v>
       </c>
@@ -2107,7 +2121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:27" s="32" customFormat="1">
+    <row r="33" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="32" t="s">
         <v>15</v>
       </c>
@@ -2118,7 +2132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:27" s="32" customFormat="1">
+    <row r="34" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="32" t="s">
         <v>15</v>
       </c>
@@ -2129,7 +2143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:27" s="32" customFormat="1">
+    <row r="35" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="32" t="s">
         <v>15</v>
       </c>
@@ -2140,7 +2154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:27" s="32" customFormat="1">
+    <row r="36" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="32" t="s">
         <v>15</v>
       </c>
@@ -2151,7 +2165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:27">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A37" s="35" t="s">
         <v>7</v>
       </c>
@@ -2187,7 +2201,7 @@
       <c r="Z37" s="32"/>
       <c r="AA37" s="32"/>
     </row>
-    <row r="38" spans="1:27">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A38" s="34" t="s">
         <v>44</v>
       </c>
@@ -2218,7 +2232,7 @@
       <c r="Z38" s="32"/>
       <c r="AA38" s="32"/>
     </row>
-    <row r="39" spans="1:27" s="32" customFormat="1">
+    <row r="39" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="32" t="s">
         <v>31</v>
       </c>
@@ -2229,7 +2243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:27" s="32" customFormat="1">
+    <row r="40" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="32" t="s">
         <v>58</v>
       </c>
@@ -2240,7 +2254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:27" s="32" customFormat="1">
+    <row r="41" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="32" t="s">
         <v>60</v>
       </c>
@@ -2252,7 +2266,7 @@
       </c>
       <c r="J41" s="33"/>
     </row>
-    <row r="42" spans="1:27" s="32" customFormat="1">
+    <row r="42" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="32" t="s">
         <v>59</v>
       </c>
@@ -2263,7 +2277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:27" s="32" customFormat="1">
+    <row r="43" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="32" t="s">
         <v>62</v>
       </c>
@@ -2274,7 +2288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:27" s="32" customFormat="1">
+    <row r="44" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="32" t="s">
         <v>61</v>
       </c>
@@ -2285,7 +2299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:27" s="32" customFormat="1">
+    <row r="45" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="32" t="s">
         <v>63</v>
       </c>
@@ -2296,7 +2310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:27" s="32" customFormat="1">
+    <row r="46" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="32" t="s">
         <v>15</v>
       </c>
@@ -2307,12 +2321,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:27" s="32" customFormat="1">
+    <row r="47" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="32" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:27" s="32" customFormat="1">
+    <row r="48" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="32" t="s">
         <v>15</v>
       </c>
@@ -2323,7 +2337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:27">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A49" s="35" t="s">
         <v>7</v>
       </c>
@@ -2359,7 +2373,7 @@
       <c r="Z49" s="32"/>
       <c r="AA49" s="32"/>
     </row>
-    <row r="50" spans="1:27">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A50" s="31" t="s">
         <v>45</v>
       </c>
@@ -2390,7 +2404,7 @@
       <c r="Z50" s="32"/>
       <c r="AA50" s="32"/>
     </row>
-    <row r="51" spans="1:27" s="32" customFormat="1">
+    <row r="51" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="32" t="s">
         <v>32</v>
       </c>
@@ -2401,74 +2415,74 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:27" s="32" customFormat="1">
+    <row r="52" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="32" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="B52" s="32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C52" s="32">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:27" s="32" customFormat="1">
+    <row r="53" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="32" t="s">
-        <v>15</v>
+        <v>69</v>
       </c>
       <c r="B53" s="32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C53" s="32">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:27" s="32" customFormat="1">
+    <row r="54" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="32" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="B54" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C54" s="32">
         <v>0</v>
       </c>
       <c r="J54" s="33"/>
     </row>
-    <row r="55" spans="1:27" s="32" customFormat="1">
+    <row r="55" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="32" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="B55" s="32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C55" s="32">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:27" s="32" customFormat="1">
+    <row r="56" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="32" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="B56" s="32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C56" s="32">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:27" s="32" customFormat="1">
+    <row r="57" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="32" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="B57" s="32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C57" s="32">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:27" s="32" customFormat="1">
+    <row r="58" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="32" t="s">
         <v>15</v>
       </c>
@@ -2479,7 +2493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:27" s="32" customFormat="1">
+    <row r="59" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="32" t="s">
         <v>15</v>
       </c>
@@ -2490,7 +2504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:27" s="32" customFormat="1">
+    <row r="60" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="32" t="s">
         <v>15</v>
       </c>
@@ -2501,13 +2515,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:27">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>7</v>
       </c>
       <c r="B61">
         <f>SUM(B51:B60)</f>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C61">
         <f>SUM(C51:C60)</f>
@@ -2537,7 +2551,7 @@
       <c r="Z61" s="32"/>
       <c r="AA61" s="32"/>
     </row>
-    <row r="62" spans="1:27">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A62" s="34" t="s">
         <v>46</v>
       </c>
@@ -2568,7 +2582,7 @@
       <c r="Z62" s="32"/>
       <c r="AA62" s="32"/>
     </row>
-    <row r="63" spans="1:27" s="32" customFormat="1">
+    <row r="63" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="32" t="s">
         <v>30</v>
       </c>
@@ -2579,7 +2593,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="64" spans="1:27" s="32" customFormat="1">
+    <row r="64" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="32" t="s">
         <v>15</v>
       </c>
@@ -2590,7 +2604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:27" s="32" customFormat="1">
+    <row r="65" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="32" t="s">
         <v>15</v>
       </c>
@@ -2601,7 +2615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:27" s="32" customFormat="1">
+    <row r="66" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="32" t="s">
         <v>15</v>
       </c>
@@ -2613,7 +2627,7 @@
       </c>
       <c r="J66" s="33"/>
     </row>
-    <row r="67" spans="1:27" s="32" customFormat="1">
+    <row r="67" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="32" t="s">
         <v>15</v>
       </c>
@@ -2624,7 +2638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:27" s="32" customFormat="1">
+    <row r="68" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="32" t="s">
         <v>15</v>
       </c>
@@ -2635,7 +2649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:27" s="32" customFormat="1">
+    <row r="69" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="32" t="s">
         <v>15</v>
       </c>
@@ -2646,7 +2660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:27" s="32" customFormat="1">
+    <row r="70" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="32" t="s">
         <v>15</v>
       </c>
@@ -2657,7 +2671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:27" s="32" customFormat="1">
+    <row r="71" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="32" t="s">
         <v>15</v>
       </c>
@@ -2668,7 +2682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:27" s="32" customFormat="1">
+    <row r="72" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="32" t="s">
         <v>15</v>
       </c>
@@ -2679,7 +2693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:27">
+    <row r="73" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>7</v>
       </c>
@@ -2715,13 +2729,13 @@
       <c r="Z73" s="32"/>
       <c r="AA73" s="32"/>
     </row>
-    <row r="74" spans="1:27">
+    <row r="74" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>16</v>
       </c>
       <c r="B74">
         <f>SUM(B13,B25,B37,B49,B61,B73)</f>
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C74">
         <f>SUM(C13,C25,C37,C49,C61,C73)</f>
@@ -2751,13 +2765,13 @@
       <c r="Z74" s="32"/>
       <c r="AA74" s="32"/>
     </row>
-    <row r="75" spans="1:27">
+    <row r="75" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>17</v>
       </c>
       <c r="B75" s="36">
         <f>B74*100</f>
-        <v>400</v>
+        <v>1700</v>
       </c>
       <c r="C75" s="36">
         <f>C74*100</f>
@@ -2771,27 +2785,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AMK10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.453125" style="37" customWidth="1"/>
-    <col min="2" max="2" width="8.81640625" style="37" customWidth="1"/>
-    <col min="3" max="3" width="7.36328125" style="37" customWidth="1"/>
-    <col min="4" max="4" width="10.6328125" style="37" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" style="37" customWidth="1"/>
-    <col min="6" max="6" width="11.36328125" style="37" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" style="37" customWidth="1"/>
-    <col min="8" max="12" width="4.1796875" style="37" bestFit="1" customWidth="1"/>
-    <col min="13" max="1025" width="8.81640625" style="37" customWidth="1"/>
+    <col min="1" max="1" width="15.5" style="37" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="37" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" style="37" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="37" customWidth="1"/>
+    <col min="5" max="5" width="9.5" style="37" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="37" customWidth="1"/>
+    <col min="7" max="7" width="10.5" style="37" customWidth="1"/>
+    <col min="8" max="12" width="4.1640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="13" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="38" t="s">
         <v>18</v>
       </c>
@@ -2829,7 +2843,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="87">
+    <row r="2" spans="1:12" ht="75" x14ac:dyDescent="0.2">
       <c r="B2" s="39" t="s">
         <v>21</v>
       </c>
@@ -2864,7 +2878,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B3" s="39" t="s">
         <v>14</v>
       </c>
@@ -2899,7 +2913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="39" t="s">
         <v>41</v>
       </c>
@@ -2926,7 +2940,7 @@
       <c r="K4" s="42"/>
       <c r="L4" s="42"/>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="39" t="s">
         <v>42</v>
       </c>
@@ -2951,7 +2965,7 @@
       <c r="K5" s="42"/>
       <c r="L5" s="42"/>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="39" t="s">
         <v>43</v>
       </c>
@@ -2980,7 +2994,7 @@
       <c r="K6" s="42"/>
       <c r="L6" s="42"/>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="39" t="s">
         <v>44</v>
       </c>
@@ -3009,7 +3023,7 @@
       <c r="K7" s="42"/>
       <c r="L7" s="42"/>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="39" t="s">
         <v>45</v>
       </c>
@@ -3038,7 +3052,7 @@
       <c r="K8" s="42"/>
       <c r="L8" s="42"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="39" t="s">
         <v>46</v>
       </c>
@@ -3067,7 +3081,7 @@
       <c r="K9" s="42"/>
       <c r="L9" s="42"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="39" t="s">
         <v>7</v>
       </c>
@@ -3123,24 +3137,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.453125" customWidth="1"/>
-    <col min="2" max="2" width="43.36328125" customWidth="1"/>
-    <col min="3" max="3" width="27.453125" customWidth="1"/>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="43.33203125" customWidth="1"/>
+    <col min="3" max="3" width="27.5" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>
-    <col min="5" max="19" width="3.6328125" customWidth="1"/>
-    <col min="20" max="1025" width="8.81640625" customWidth="1"/>
+    <col min="5" max="19" width="3.6640625" customWidth="1"/>
+    <col min="20" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="43"/>
       <c r="B1" s="44" t="s">
         <v>22</v>
@@ -3197,7 +3211,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>41</v>
       </c>
@@ -3222,7 +3236,7 @@
       <c r="N2" s="32"/>
       <c r="O2" s="32"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="49"/>
       <c r="B3" s="46" t="s">
         <v>36</v>
@@ -3245,7 +3259,7 @@
       <c r="N3" s="32"/>
       <c r="O3" s="32"/>
     </row>
-    <row r="4" spans="1:19" s="32" customFormat="1">
+    <row r="4" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="49"/>
       <c r="B4" s="46" t="s">
         <v>25</v>
@@ -3258,7 +3272,7 @@
       </c>
       <c r="J4" s="50"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="46" t="s">
         <v>23</v>
@@ -3283,7 +3297,7 @@
       <c r="N5" s="32"/>
       <c r="O5" s="32"/>
     </row>
-    <row r="6" spans="1:19" s="32" customFormat="1">
+    <row r="6" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>42</v>
       </c>
@@ -3297,7 +3311,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="32" customFormat="1">
+    <row r="7" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="49"/>
       <c r="B7" s="46" t="s">
         <v>39</v>
@@ -3310,7 +3324,7 @@
       </c>
       <c r="J7" s="50"/>
     </row>
-    <row r="8" spans="1:19" s="32" customFormat="1">
+    <row r="8" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="49"/>
       <c r="B8" s="46" t="s">
         <v>25</v>
@@ -3323,7 +3337,7 @@
       </c>
       <c r="J8" s="50"/>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="49"/>
       <c r="B9" s="46" t="s">
         <v>23</v>
@@ -3348,7 +3362,7 @@
       <c r="N9" s="32"/>
       <c r="O9" s="32"/>
     </row>
-    <row r="10" spans="1:19" s="32" customFormat="1">
+    <row r="10" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>43</v>
       </c>
@@ -3362,7 +3376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="32" customFormat="1">
+    <row r="11" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="49"/>
       <c r="B11" s="46" t="s">
         <v>38</v>
@@ -3375,7 +3389,7 @@
       </c>
       <c r="J11" s="50"/>
     </row>
-    <row r="12" spans="1:19" s="32" customFormat="1">
+    <row r="12" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="49"/>
       <c r="B12" s="46" t="s">
         <v>25</v>
@@ -3388,7 +3402,7 @@
       </c>
       <c r="J12" s="50"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="49"/>
       <c r="B13" s="52" t="s">
         <v>23</v>
@@ -3413,7 +3427,7 @@
       <c r="N13" s="32"/>
       <c r="O13" s="32"/>
     </row>
-    <row r="14" spans="1:19" s="32" customFormat="1">
+    <row r="14" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>44</v>
       </c>
@@ -3427,7 +3441,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:19" s="32" customFormat="1">
+    <row r="15" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="49"/>
       <c r="B15" s="46" t="s">
         <v>35</v>
@@ -3440,7 +3454,7 @@
       </c>
       <c r="J15" s="50"/>
     </row>
-    <row r="16" spans="1:19" s="32" customFormat="1">
+    <row r="16" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="49"/>
       <c r="B16" s="46" t="s">
         <v>25</v>
@@ -3453,7 +3467,7 @@
       </c>
       <c r="J16" s="50"/>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="49"/>
       <c r="B17" s="46" t="s">
         <v>23</v>
@@ -3478,7 +3492,7 @@
       <c r="N17" s="32"/>
       <c r="O17" s="32"/>
     </row>
-    <row r="18" spans="1:15" s="32" customFormat="1">
+    <row r="18" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>45</v>
       </c>
@@ -3492,7 +3506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15" s="32" customFormat="1">
+    <row r="19" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="49"/>
       <c r="B19" s="46" t="s">
         <v>37</v>
@@ -3505,7 +3519,7 @@
       </c>
       <c r="J19" s="50"/>
     </row>
-    <row r="20" spans="1:15" s="32" customFormat="1">
+    <row r="20" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="49"/>
       <c r="B20" s="46" t="s">
         <v>25</v>
@@ -3518,7 +3532,7 @@
       </c>
       <c r="J20" s="50"/>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="49"/>
       <c r="B21" s="52" t="s">
         <v>23</v>
@@ -3543,7 +3557,7 @@
       <c r="N21" s="32"/>
       <c r="O21" s="32"/>
     </row>
-    <row r="22" spans="1:15" s="32" customFormat="1">
+    <row r="22" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
         <v>46</v>
       </c>
@@ -3557,7 +3571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="32" customFormat="1">
+    <row r="23" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="49"/>
       <c r="B23" s="46" t="s">
         <v>34</v>
@@ -3570,7 +3584,7 @@
       </c>
       <c r="J23" s="50"/>
     </row>
-    <row r="24" spans="1:15" s="32" customFormat="1">
+    <row r="24" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="49"/>
       <c r="B24" s="46" t="s">
         <v>25</v>
@@ -3583,7 +3597,7 @@
       </c>
       <c r="J24" s="50"/>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="49"/>
       <c r="B25" s="52" t="s">
         <v>24</v>
@@ -3608,7 +3622,7 @@
       <c r="N25" s="32"/>
       <c r="O25" s="32"/>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="53"/>
       <c r="B26" s="54" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Updated master gantt and file name changed
</commit_message>
<xml_diff>
--- a/Documents/Master Gantt.xlsx
+++ b/Documents/Master Gantt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\Documents\GitHub\Maze_Runner\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BenjaminHallman/Documents/College/Classes/Computer Science/383/Projects/Dream Team/Maze Runner/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E901201-88BB-4561-8612-F0E142342074}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4416ED97-839A-034C-8701-169B9F244EB2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16890" yWindow="2310" windowWidth="28800" windowHeight="15435" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Management Summary" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="88">
   <si>
     <t>Total</t>
   </si>
@@ -226,9 +226,6 @@
   </si>
   <si>
     <t>Presentation Rehersal</t>
-  </si>
-  <si>
-    <t>TDB</t>
   </si>
   <si>
     <r>
@@ -319,6 +316,12 @@
   </si>
   <si>
     <t>Implement Scene Swapper</t>
+  </si>
+  <si>
+    <t>Development and Merging</t>
+  </si>
+  <si>
+    <t>Feb. 26</t>
   </si>
 </sst>
 </file>
@@ -363,7 +366,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -416,6 +419,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor rgb="FF993300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
   </fills>
@@ -561,7 +576,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -642,7 +657,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -672,11 +686,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1027,53 +1044,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="3.42578125" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="2.85546875" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="3.5" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="8" max="8" width="14.5" customWidth="1"/>
+    <col min="9" max="9" width="2.83203125" customWidth="1"/>
+    <col min="10" max="10" width="13.83203125" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" customWidth="1"/>
-    <col min="13" max="13" width="5.42578125" customWidth="1"/>
-    <col min="14" max="14" width="12.28515625" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" customWidth="1"/>
-    <col min="16" max="16" width="11.28515625" customWidth="1"/>
-    <col min="17" max="1025" width="8.85546875" customWidth="1"/>
+    <col min="12" max="12" width="14.1640625" customWidth="1"/>
+    <col min="13" max="13" width="5.5" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" customWidth="1"/>
+    <col min="15" max="15" width="14.6640625" customWidth="1"/>
+    <col min="16" max="16" width="11.33203125" customWidth="1"/>
+    <col min="17" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
-      <c r="B1" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
+      <c r="B1" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="54" t="s">
+      <c r="F1" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="J1" s="54" t="s">
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="J1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="N1" s="54" t="s">
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="N1" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
     </row>
     <row r="2" spans="1:16">
       <c r="B2" s="2" t="s">
@@ -1126,11 +1143,11 @@
       </c>
       <c r="C3" s="11">
         <f t="shared" si="0"/>
-        <v>2125</v>
+        <v>2425</v>
       </c>
       <c r="D3" s="12">
         <f t="shared" ref="D3:D8" si="1">(B3-C3)</f>
-        <v>4975</v>
+        <v>4675</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="13">
@@ -1151,11 +1168,11 @@
       </c>
       <c r="K3" s="11">
         <f>Meetings!B4*100</f>
-        <v>875</v>
+        <v>1175</v>
       </c>
       <c r="L3" s="12">
         <f t="shared" ref="L3:L8" si="3">(J3-K3)</f>
-        <v>625</v>
+        <v>325</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="10">
@@ -1181,11 +1198,11 @@
       </c>
       <c r="C4" s="14">
         <f t="shared" si="0"/>
-        <v>1675</v>
+        <v>1975</v>
       </c>
       <c r="D4" s="15">
         <f t="shared" si="1"/>
-        <v>925</v>
+        <v>625</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="13">
@@ -1206,11 +1223,11 @@
       </c>
       <c r="K4" s="14">
         <f>Meetings!B5*100</f>
-        <v>875</v>
+        <v>1175</v>
       </c>
       <c r="L4" s="15">
         <f t="shared" si="3"/>
-        <v>625</v>
+        <v>325</v>
       </c>
       <c r="M4" s="5"/>
       <c r="N4" s="13">
@@ -1236,11 +1253,11 @@
       </c>
       <c r="C5" s="14">
         <f t="shared" si="0"/>
-        <v>925</v>
+        <v>1225</v>
       </c>
       <c r="D5" s="15">
         <f t="shared" si="1"/>
-        <v>1675</v>
+        <v>1375</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="13">
@@ -1261,11 +1278,11 @@
       </c>
       <c r="K5" s="14">
         <f>Meetings!B6*100</f>
-        <v>925</v>
+        <v>1225</v>
       </c>
       <c r="L5" s="15">
         <f t="shared" si="3"/>
-        <v>575</v>
+        <v>275</v>
       </c>
       <c r="M5" s="5"/>
       <c r="N5" s="13">
@@ -1291,11 +1308,11 @@
       </c>
       <c r="C6" s="14">
         <f t="shared" si="0"/>
-        <v>2175</v>
+        <v>3775</v>
       </c>
       <c r="D6" s="15">
         <f t="shared" si="1"/>
-        <v>3925</v>
+        <v>2325</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="13">
@@ -1304,11 +1321,11 @@
       </c>
       <c r="G6" s="14">
         <f>(Gantt!$C49)*100</f>
-        <v>100</v>
+        <v>1400</v>
       </c>
       <c r="H6" s="15">
         <f t="shared" si="2"/>
-        <v>3000</v>
+        <v>1700</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="13">
@@ -1316,11 +1333,11 @@
       </c>
       <c r="K6" s="14">
         <f>Meetings!B7*100</f>
-        <v>925</v>
+        <v>1225</v>
       </c>
       <c r="L6" s="15">
         <f t="shared" si="3"/>
-        <v>575</v>
+        <v>275</v>
       </c>
       <c r="M6" s="5"/>
       <c r="N6" s="13">
@@ -1401,11 +1418,11 @@
       </c>
       <c r="C8" s="18">
         <f t="shared" si="0"/>
-        <v>2395</v>
+        <v>2695</v>
       </c>
       <c r="D8" s="19">
         <f t="shared" si="1"/>
-        <v>3705</v>
+        <v>3405</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="13">
@@ -1426,11 +1443,11 @@
       </c>
       <c r="K8" s="14">
         <f>Meetings!B9*100</f>
-        <v>925</v>
+        <v>1225</v>
       </c>
       <c r="L8" s="15">
         <f t="shared" si="3"/>
-        <v>575</v>
+        <v>275</v>
       </c>
       <c r="M8" s="5"/>
       <c r="N8" s="17">
@@ -1456,11 +1473,11 @@
       </c>
       <c r="C9" s="22">
         <f>SUM(C3:C8)</f>
-        <v>11320</v>
+        <v>14120</v>
       </c>
       <c r="D9" s="23">
         <f>SUM(D3:D8)</f>
-        <v>15880</v>
+        <v>13080</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="24">
@@ -1469,11 +1486,11 @@
       </c>
       <c r="G9" s="25">
         <f>SUM(G3:G8)</f>
-        <v>370</v>
+        <v>1670</v>
       </c>
       <c r="H9" s="26">
         <f>SUM(H3:H8)</f>
-        <v>10630</v>
+        <v>9330</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="24">
@@ -1482,11 +1499,11 @@
       </c>
       <c r="K9" s="25">
         <f>SUM(K3:K8)</f>
-        <v>5450</v>
+        <v>6950</v>
       </c>
       <c r="L9" s="26">
         <f>SUM(L3:L8)</f>
-        <v>3550</v>
+        <v>2050</v>
       </c>
       <c r="M9" s="5"/>
       <c r="N9" s="21">
@@ -1518,19 +1535,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AU75"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="AD23" sqref="AD23"/>
+    <sheetView topLeftCell="A25" zoomScale="116" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" customWidth="1"/>
-    <col min="7" max="1025" width="8.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="7.5" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" customWidth="1"/>
+    <col min="6" max="6" width="9.5" customWidth="1"/>
+    <col min="7" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:47">
@@ -1574,11 +1591,11 @@
       <c r="C3">
         <v>0.5</v>
       </c>
-      <c r="E3" s="55"/>
+      <c r="E3" s="53"/>
     </row>
     <row r="4" spans="1:47">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -1586,15 +1603,15 @@
       <c r="C4">
         <v>0</v>
       </c>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
     </row>
     <row r="5" spans="1:47">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -1602,13 +1619,13 @@
       <c r="C5">
         <v>0</v>
       </c>
-      <c r="K5" s="56"/>
-      <c r="L5" s="56"/>
-      <c r="M5" s="56"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="54"/>
     </row>
     <row r="6" spans="1:47">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B6">
         <v>15</v>
@@ -1617,25 +1634,25 @@
         <v>0</v>
       </c>
       <c r="J6" s="31"/>
-      <c r="N6" s="56"/>
-      <c r="O6" s="56"/>
-      <c r="P6" s="56"/>
-      <c r="Q6" s="56"/>
-      <c r="R6" s="56"/>
-      <c r="S6" s="56"/>
-      <c r="T6" s="56"/>
-      <c r="U6" s="56"/>
-      <c r="V6" s="56"/>
-      <c r="W6" s="56"/>
-      <c r="X6" s="56"/>
-      <c r="Y6" s="56"/>
-      <c r="Z6" s="56"/>
-      <c r="AA6" s="56"/>
-      <c r="AB6" s="56"/>
+      <c r="N6" s="54"/>
+      <c r="O6" s="54"/>
+      <c r="P6" s="54"/>
+      <c r="Q6" s="54"/>
+      <c r="R6" s="54"/>
+      <c r="S6" s="54"/>
+      <c r="T6" s="54"/>
+      <c r="U6" s="54"/>
+      <c r="V6" s="54"/>
+      <c r="W6" s="54"/>
+      <c r="X6" s="54"/>
+      <c r="Y6" s="54"/>
+      <c r="Z6" s="54"/>
+      <c r="AA6" s="54"/>
+      <c r="AB6" s="54"/>
     </row>
     <row r="7" spans="1:47">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B7">
         <v>10</v>
@@ -1643,20 +1660,20 @@
       <c r="C7">
         <v>0</v>
       </c>
-      <c r="AC7" s="56"/>
-      <c r="AD7" s="56"/>
-      <c r="AE7" s="56"/>
-      <c r="AF7" s="56"/>
-      <c r="AG7" s="56"/>
-      <c r="AH7" s="56"/>
-      <c r="AI7" s="56"/>
-      <c r="AJ7" s="56"/>
-      <c r="AK7" s="56"/>
-      <c r="AL7" s="56"/>
+      <c r="AC7" s="54"/>
+      <c r="AD7" s="54"/>
+      <c r="AE7" s="54"/>
+      <c r="AF7" s="54"/>
+      <c r="AG7" s="54"/>
+      <c r="AH7" s="54"/>
+      <c r="AI7" s="54"/>
+      <c r="AJ7" s="54"/>
+      <c r="AK7" s="54"/>
+      <c r="AL7" s="54"/>
     </row>
     <row r="8" spans="1:47">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -1664,12 +1681,12 @@
       <c r="C8">
         <v>0</v>
       </c>
-      <c r="AM8" s="56"/>
-      <c r="AN8" s="56"/>
+      <c r="AM8" s="54"/>
+      <c r="AN8" s="54"/>
     </row>
     <row r="9" spans="1:47">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1677,7 +1694,7 @@
       <c r="C9">
         <v>0</v>
       </c>
-      <c r="AO9" s="56"/>
+      <c r="AO9" s="54"/>
     </row>
     <row r="10" spans="1:47">
       <c r="A10" t="s">
@@ -1689,11 +1706,11 @@
       <c r="C10">
         <v>0</v>
       </c>
-      <c r="AP10" s="56"/>
-      <c r="AQ10" s="56"/>
-      <c r="AR10" s="56"/>
-      <c r="AS10" s="56"/>
-      <c r="AT10" s="56"/>
+      <c r="AP10" s="54"/>
+      <c r="AQ10" s="54"/>
+      <c r="AR10" s="54"/>
+      <c r="AS10" s="54"/>
+      <c r="AT10" s="54"/>
     </row>
     <row r="11" spans="1:47">
       <c r="A11" t="s">
@@ -1705,7 +1722,7 @@
       <c r="C11">
         <v>0</v>
       </c>
-      <c r="AU11" s="56"/>
+      <c r="AU11" s="54"/>
     </row>
     <row r="12" spans="1:47">
       <c r="A12" t="s">
@@ -2023,11 +2040,11 @@
         <v>3</v>
       </c>
       <c r="C40">
-        <v>0</v>
-      </c>
-      <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="29"/>
+        <v>3</v>
+      </c>
+      <c r="F40" s="56"/>
+      <c r="G40" s="56"/>
+      <c r="H40" s="56"/>
     </row>
     <row r="41" spans="1:35">
       <c r="A41" t="s">
@@ -2037,14 +2054,14 @@
         <v>6</v>
       </c>
       <c r="C41">
-        <v>0</v>
-      </c>
-      <c r="I41" s="29"/>
-      <c r="J41" s="34"/>
-      <c r="K41" s="29"/>
-      <c r="L41" s="29"/>
-      <c r="M41" s="29"/>
-      <c r="N41" s="29"/>
+        <v>6</v>
+      </c>
+      <c r="I41" s="56"/>
+      <c r="J41" s="57"/>
+      <c r="K41" s="56"/>
+      <c r="L41" s="56"/>
+      <c r="M41" s="56"/>
+      <c r="N41" s="56"/>
     </row>
     <row r="42" spans="1:35">
       <c r="A42" t="s">
@@ -2054,14 +2071,14 @@
         <v>6</v>
       </c>
       <c r="C42">
-        <v>0</v>
-      </c>
-      <c r="O42" s="29"/>
-      <c r="P42" s="29"/>
-      <c r="Q42" s="29"/>
-      <c r="R42" s="29"/>
-      <c r="S42" s="29"/>
-      <c r="T42" s="29"/>
+        <v>4</v>
+      </c>
+      <c r="O42" s="56"/>
+      <c r="P42" s="56"/>
+      <c r="Q42" s="56"/>
+      <c r="R42" s="56"/>
+      <c r="S42" s="56"/>
+      <c r="T42" s="56"/>
     </row>
     <row r="43" spans="1:35">
       <c r="A43" t="s">
@@ -2073,12 +2090,12 @@
       <c r="C43">
         <v>0</v>
       </c>
-      <c r="U43" s="29"/>
-      <c r="V43" s="29"/>
-      <c r="W43" s="29"/>
-      <c r="X43" s="29"/>
-      <c r="Y43" s="29"/>
-      <c r="Z43" s="29"/>
+      <c r="U43" s="58"/>
+      <c r="V43" s="58"/>
+      <c r="W43" s="58"/>
+      <c r="X43" s="58"/>
+      <c r="Y43" s="58"/>
+      <c r="Z43" s="58"/>
     </row>
     <row r="44" spans="1:35">
       <c r="A44" t="s">
@@ -2154,7 +2171,7 @@
       </c>
       <c r="C49">
         <f>SUM(C39:C48)</f>
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -2431,20 +2448,20 @@
       </c>
       <c r="C74">
         <f>SUM(C13,C25,C37,C49,C61,C73)</f>
-        <v>3.7</v>
+        <v>16.7</v>
       </c>
     </row>
     <row r="75" spans="1:10">
       <c r="A75" t="s">
         <v>46</v>
       </c>
-      <c r="B75" s="35">
+      <c r="B75" s="34">
         <f>B74*100</f>
         <v>11000</v>
       </c>
-      <c r="C75" s="35">
+      <c r="C75" s="34">
         <f>C74*100</f>
-        <v>370</v>
+        <v>1670</v>
       </c>
     </row>
   </sheetData>
@@ -2458,27 +2475,28 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="36" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="36" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" style="36" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="36" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="36" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="36" customWidth="1"/>
-    <col min="7" max="8" width="10.42578125" style="36" customWidth="1"/>
-    <col min="9" max="12" width="4.140625" style="36" customWidth="1"/>
-    <col min="13" max="1025" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.5" style="35" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="35" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" style="35" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="35" customWidth="1"/>
+    <col min="5" max="5" width="9.5" style="35" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="35" customWidth="1"/>
+    <col min="7" max="8" width="10.5" style="35" customWidth="1"/>
+    <col min="9" max="9" width="11" style="35" customWidth="1"/>
+    <col min="10" max="12" width="4.1640625" style="35" customWidth="1"/>
+    <col min="13" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="38" t="s">
+      <c r="A1" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="37" t="s">
         <v>48</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -2500,7 +2518,7 @@
         <v>54</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>22</v>
+        <v>87</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>22</v>
@@ -2512,43 +2530,43 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="90">
-      <c r="B2" s="38" t="s">
+    <row r="2" spans="1:12" ht="128">
+      <c r="B2" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="39" t="s">
+      <c r="G2" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="H2" s="39" t="s">
+      <c r="H2" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="J2" s="39" t="s">
+      <c r="I2" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="39" t="s">
+      <c r="K2" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="39" t="s">
+      <c r="L2" s="38" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="37" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="3">
@@ -2570,7 +2588,7 @@
         <v>1.5</v>
       </c>
       <c r="I3" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J3" s="3">
         <v>0</v>
@@ -2583,193 +2601,204 @@
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="38">
+      <c r="B4" s="37">
         <f t="shared" ref="B4:B9" si="0">SUMIF(C4:L4,A$1,C$3:Z$3)</f>
-        <v>8.75</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="40"/>
-      <c r="E4" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="G4" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="H4" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
+        <v>11.75</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="39"/>
+      <c r="E4" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="38">
+      <c r="B5" s="37">
         <f t="shared" si="0"/>
-        <v>8.75</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="40"/>
-      <c r="E5" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="H5" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
+        <v>11.75</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="39"/>
+      <c r="E5" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="38">
+      <c r="B6" s="37">
+        <f t="shared" si="0"/>
+        <v>12.25</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="39"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="37">
+        <f t="shared" si="0"/>
+        <v>12.25</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="39"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="37">
         <f t="shared" si="0"/>
         <v>9.25</v>
       </c>
-      <c r="C6" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="H6" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="38">
+      <c r="C8" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="I8" s="39"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="37">
         <f t="shared" si="0"/>
-        <v>9.25</v>
-      </c>
-      <c r="C7" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="H7" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="I7" s="40"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="40"/>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="38">
-        <f t="shared" si="0"/>
-        <v>9.25</v>
-      </c>
-      <c r="C8" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="G8" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="H8" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="I8" s="40"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="40"/>
-      <c r="L8" s="40"/>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="38">
-        <f t="shared" si="0"/>
-        <v>9.25</v>
-      </c>
-      <c r="C9" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="H9" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="I9" s="40"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="40"/>
-      <c r="L9" s="40"/>
+        <v>12.25</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="I9" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="39"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="38">
+      <c r="B10" s="37">
         <f>SUM(B4:B9)</f>
-        <v>54.5</v>
+        <v>69.5</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ref="C10:L10" si="1">COUNTIF(C4:C9,"*ü*") * C3</f>
@@ -2797,7 +2826,7 @@
       </c>
       <c r="I10" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J10" s="3">
         <f t="shared" si="1"/>
@@ -2822,29 +2851,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="43.28515625" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="43.33203125" customWidth="1"/>
+    <col min="3" max="3" width="27.5" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>
-    <col min="5" max="19" width="3.7109375" customWidth="1"/>
-    <col min="20" max="1025" width="8.85546875" customWidth="1"/>
+    <col min="5" max="19" width="3.6640625" customWidth="1"/>
+    <col min="20" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="41"/>
-      <c r="B1" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" s="42" t="s">
+      <c r="A1" s="40"/>
+      <c r="B1" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="42" t="s">
         <v>15</v>
       </c>
       <c r="E1">
@@ -2897,78 +2926,78 @@
       <c r="A2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="44" t="s">
-        <v>64</v>
+      <c r="B2" s="43" t="s">
+        <v>63</v>
       </c>
       <c r="C2">
         <v>6</v>
       </c>
-      <c r="D2" s="45">
+      <c r="D2" s="44">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:19">
-      <c r="A3" s="46"/>
-      <c r="B3" s="44" t="s">
-        <v>65</v>
+      <c r="A3" s="45"/>
+      <c r="B3" s="43" t="s">
+        <v>64</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
-      <c r="D3" s="45">
+      <c r="D3" s="44">
         <v>1</v>
       </c>
-      <c r="J3" s="47"/>
+      <c r="J3" s="46"/>
     </row>
     <row r="4" spans="1:19">
-      <c r="A4" s="46"/>
-      <c r="B4" s="44" t="s">
-        <v>66</v>
+      <c r="A4" s="45"/>
+      <c r="B4" s="43" t="s">
+        <v>65</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
-      <c r="D4" s="45">
+      <c r="D4" s="44">
         <v>2</v>
       </c>
-      <c r="J4" s="47"/>
+      <c r="J4" s="46"/>
     </row>
     <row r="5" spans="1:19">
-      <c r="A5" s="46"/>
-      <c r="B5" s="44" t="s">
-        <v>79</v>
+      <c r="A5" s="45"/>
+      <c r="B5" s="43" t="s">
+        <v>78</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="45">
+      <c r="D5" s="44">
         <v>1</v>
       </c>
-      <c r="J5" s="47"/>
+      <c r="J5" s="46"/>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="46"/>
-      <c r="B6" s="44" t="s">
-        <v>80</v>
+      <c r="A6" s="45"/>
+      <c r="B6" s="43" t="s">
+        <v>79</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" s="45">
+      <c r="D6" s="44">
         <v>1</v>
       </c>
-      <c r="J6" s="47"/>
+      <c r="J6" s="46"/>
     </row>
     <row r="7" spans="1:19">
-      <c r="A7" s="46"/>
-      <c r="B7" s="44" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7" s="44">
+      <c r="A7" s="45"/>
+      <c r="B7" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="43">
         <f>SUM(C2:C6)</f>
         <v>13</v>
       </c>
-      <c r="D7" s="48">
+      <c r="D7" s="47">
         <f>SUM(D2:D6)</f>
         <v>12</v>
       </c>
@@ -2977,78 +3006,78 @@
       <c r="A8" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="44" t="s">
-        <v>68</v>
+      <c r="B8" s="43" t="s">
+        <v>67</v>
       </c>
       <c r="C8">
         <v>6</v>
       </c>
-      <c r="D8" s="45">
+      <c r="D8" s="44">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:19">
-      <c r="A9" s="46"/>
-      <c r="B9" s="44" t="s">
-        <v>69</v>
+      <c r="A9" s="45"/>
+      <c r="B9" s="43" t="s">
+        <v>68</v>
       </c>
       <c r="C9">
         <v>3</v>
       </c>
-      <c r="D9" s="45">
+      <c r="D9" s="44">
         <v>1</v>
       </c>
-      <c r="J9" s="47"/>
+      <c r="J9" s="46"/>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="46"/>
-      <c r="B10" s="44" t="s">
-        <v>66</v>
+      <c r="A10" s="45"/>
+      <c r="B10" s="43" t="s">
+        <v>65</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
-      <c r="D10" s="45">
+      <c r="D10" s="44">
         <v>1</v>
       </c>
-      <c r="J10" s="47"/>
+      <c r="J10" s="46"/>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="46"/>
-      <c r="B11" s="44" t="s">
+      <c r="A11" s="45"/>
+      <c r="B11" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" s="44">
+        <v>0</v>
+      </c>
+      <c r="J11" s="46"/>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" s="45"/>
+      <c r="B12" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11" s="45">
-        <v>0</v>
-      </c>
-      <c r="J11" s="47"/>
-    </row>
-    <row r="12" spans="1:19">
-      <c r="A12" s="46"/>
-      <c r="B12" s="44" t="s">
-        <v>80</v>
-      </c>
       <c r="C12">
         <v>0</v>
       </c>
-      <c r="D12" s="45">
-        <v>0</v>
-      </c>
-      <c r="J12" s="47"/>
+      <c r="D12" s="44">
+        <v>0</v>
+      </c>
+      <c r="J12" s="46"/>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" s="46"/>
-      <c r="B13" s="44" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" s="44">
+      <c r="A13" s="45"/>
+      <c r="B13" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="43">
         <f>SUM(C8:C12)</f>
         <v>11</v>
       </c>
-      <c r="D13" s="48">
+      <c r="D13" s="47">
         <f>SUM(D8:D12)</f>
         <v>8</v>
       </c>
@@ -3057,332 +3086,347 @@
       <c r="A14" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="44" t="s">
-        <v>70</v>
+      <c r="B14" s="43" t="s">
+        <v>69</v>
       </c>
       <c r="C14">
         <v>6</v>
       </c>
-      <c r="D14" s="45">
+      <c r="D14" s="44">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="46"/>
-      <c r="B15" s="44" t="s">
-        <v>71</v>
+      <c r="A15" s="45"/>
+      <c r="B15" s="43" t="s">
+        <v>70</v>
       </c>
       <c r="C15">
         <v>3</v>
       </c>
-      <c r="D15" s="45">
-        <v>0</v>
-      </c>
-      <c r="J15" s="47"/>
+      <c r="D15" s="44">
+        <v>0</v>
+      </c>
+      <c r="J15" s="46"/>
     </row>
     <row r="16" spans="1:19">
-      <c r="A16" s="46"/>
-      <c r="B16" s="44" t="s">
-        <v>66</v>
+      <c r="A16" s="45"/>
+      <c r="B16" s="43" t="s">
+        <v>65</v>
       </c>
       <c r="C16">
         <v>2</v>
       </c>
-      <c r="D16" s="45">
-        <v>0</v>
-      </c>
-      <c r="J16" s="47"/>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="46"/>
-      <c r="B17" s="44" t="s">
+      <c r="D16" s="44">
+        <v>0</v>
+      </c>
+      <c r="J16" s="46"/>
+    </row>
+    <row r="17" spans="1:19">
+      <c r="A17" s="45"/>
+      <c r="B17" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17" s="44">
+        <v>0</v>
+      </c>
+      <c r="J17" s="46"/>
+    </row>
+    <row r="18" spans="1:19">
+      <c r="A18" s="45"/>
+      <c r="B18" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17" s="45">
-        <v>0</v>
-      </c>
-      <c r="J17" s="47"/>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="46"/>
-      <c r="B18" s="44" t="s">
-        <v>80</v>
-      </c>
       <c r="C18">
         <v>0</v>
       </c>
-      <c r="D18" s="45">
-        <v>0</v>
-      </c>
-      <c r="J18" s="47"/>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="46"/>
-      <c r="B19" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="C19" s="44">
+      <c r="D18" s="44">
+        <v>0</v>
+      </c>
+      <c r="J18" s="46"/>
+    </row>
+    <row r="19" spans="1:19">
+      <c r="A19" s="45"/>
+      <c r="B19" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="43">
         <f>SUM(C14:C18)</f>
         <v>11</v>
       </c>
-      <c r="D19" s="48">
+      <c r="D19" s="47">
         <f>SUM(D14:D18)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:19">
       <c r="A20" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="44" t="s">
-        <v>72</v>
+      <c r="B20" s="43" t="s">
+        <v>71</v>
       </c>
       <c r="C20">
         <v>6</v>
       </c>
-      <c r="D20" s="45">
+      <c r="D20" s="44">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="46"/>
-      <c r="B21" s="44" t="s">
-        <v>73</v>
+      <c r="E20" s="53"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
+    </row>
+    <row r="21" spans="1:19">
+      <c r="A21" s="45"/>
+      <c r="B21" s="43" t="s">
+        <v>72</v>
       </c>
       <c r="C21">
         <v>3</v>
       </c>
-      <c r="D21" s="45">
+      <c r="D21" s="44">
         <v>1.5</v>
       </c>
-      <c r="J21" s="47"/>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="46"/>
-      <c r="B22" s="44" t="s">
-        <v>66</v>
+      <c r="J21" s="46"/>
+      <c r="K21" s="53"/>
+      <c r="L21" s="53"/>
+      <c r="M21" s="53"/>
+    </row>
+    <row r="22" spans="1:19">
+      <c r="A22" s="45"/>
+      <c r="B22" s="43" t="s">
+        <v>65</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
-      <c r="D22" s="45">
+      <c r="D22" s="44">
         <v>2</v>
       </c>
-      <c r="J22" s="47"/>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="46"/>
-      <c r="B23" s="44" t="s">
-        <v>79</v>
+      <c r="J22" s="46"/>
+      <c r="N22" s="53"/>
+      <c r="O22" s="53"/>
+    </row>
+    <row r="23" spans="1:19">
+      <c r="A23" s="45"/>
+      <c r="B23" s="43" t="s">
+        <v>78</v>
       </c>
       <c r="C23">
         <v>2</v>
       </c>
-      <c r="D23" s="45">
+      <c r="D23" s="44">
         <v>1.5</v>
       </c>
-      <c r="J23" s="47"/>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="46"/>
-      <c r="B24" s="44" t="s">
-        <v>80</v>
+      <c r="J23" s="46"/>
+      <c r="P23" s="53"/>
+      <c r="Q23" s="53"/>
+    </row>
+    <row r="24" spans="1:19">
+      <c r="A24" s="45"/>
+      <c r="B24" s="43" t="s">
+        <v>79</v>
       </c>
       <c r="C24">
         <v>2</v>
       </c>
-      <c r="D24" s="45">
+      <c r="D24" s="44">
         <v>1.5</v>
       </c>
-      <c r="J24" s="47"/>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="46"/>
-      <c r="B25" s="44" t="s">
-        <v>67</v>
-      </c>
-      <c r="C25" s="44">
+      <c r="J24" s="46"/>
+      <c r="R24" s="53"/>
+      <c r="S24" s="53"/>
+    </row>
+    <row r="25" spans="1:19">
+      <c r="A25" s="45"/>
+      <c r="B25" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="43">
         <f>SUM(C20:C24)</f>
         <v>15</v>
       </c>
-      <c r="D25" s="48">
+      <c r="D25" s="47">
         <f>SUM(D20:D24)</f>
         <v>11.5</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:19">
       <c r="A26" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="44" t="s">
-        <v>74</v>
+      <c r="B26" s="43" t="s">
+        <v>73</v>
       </c>
       <c r="C26">
         <v>6</v>
       </c>
-      <c r="D26" s="45">
+      <c r="D26" s="44">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="46"/>
-      <c r="B27" s="44" t="s">
-        <v>75</v>
+    <row r="27" spans="1:19">
+      <c r="A27" s="45"/>
+      <c r="B27" s="43" t="s">
+        <v>74</v>
       </c>
       <c r="C27">
         <v>3</v>
       </c>
-      <c r="D27" s="45">
+      <c r="D27" s="44">
         <v>1</v>
       </c>
-      <c r="J27" s="47"/>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="46"/>
-      <c r="B28" s="44" t="s">
-        <v>66</v>
+      <c r="J27" s="46"/>
+    </row>
+    <row r="28" spans="1:19">
+      <c r="A28" s="45"/>
+      <c r="B28" s="43" t="s">
+        <v>65</v>
       </c>
       <c r="C28">
         <v>2</v>
       </c>
-      <c r="D28" s="45">
+      <c r="D28" s="44">
         <v>2</v>
       </c>
-      <c r="J28" s="47"/>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="46"/>
-      <c r="B29" s="44" t="s">
+      <c r="J28" s="46"/>
+    </row>
+    <row r="29" spans="1:19">
+      <c r="A29" s="45"/>
+      <c r="B29" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29" s="44">
+        <v>0</v>
+      </c>
+      <c r="J29" s="46"/>
+    </row>
+    <row r="30" spans="1:19">
+      <c r="A30" s="45"/>
+      <c r="B30" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29" s="45">
-        <v>0</v>
-      </c>
-      <c r="J29" s="47"/>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30" s="46"/>
-      <c r="B30" s="44" t="s">
-        <v>80</v>
-      </c>
       <c r="C30">
         <v>0</v>
       </c>
-      <c r="D30" s="45">
-        <v>0</v>
-      </c>
-      <c r="J30" s="47"/>
-    </row>
-    <row r="31" spans="1:10">
-      <c r="A31" s="46"/>
-      <c r="B31" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="C31" s="44">
+      <c r="D30" s="44">
+        <v>0</v>
+      </c>
+      <c r="J30" s="46"/>
+    </row>
+    <row r="31" spans="1:19">
+      <c r="A31" s="45"/>
+      <c r="B31" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="43">
         <f>SUM(C26:C30)</f>
         <v>11</v>
       </c>
-      <c r="D31" s="48">
+      <c r="D31" s="47">
         <f>SUM(D26:D30)</f>
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:19">
       <c r="A32" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="44" t="s">
-        <v>76</v>
+      <c r="B32" s="43" t="s">
+        <v>75</v>
       </c>
       <c r="C32">
         <v>6</v>
       </c>
-      <c r="D32" s="45">
+      <c r="D32" s="44">
         <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="46"/>
-      <c r="B33" s="44" t="s">
-        <v>77</v>
+      <c r="A33" s="45"/>
+      <c r="B33" s="43" t="s">
+        <v>76</v>
       </c>
       <c r="C33">
         <v>3</v>
       </c>
-      <c r="D33" s="45">
+      <c r="D33" s="44">
         <v>0.5</v>
       </c>
-      <c r="J33" s="47"/>
+      <c r="J33" s="46"/>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="46"/>
-      <c r="B34" s="44" t="s">
-        <v>66</v>
+      <c r="A34" s="45"/>
+      <c r="B34" s="43" t="s">
+        <v>65</v>
       </c>
       <c r="C34">
         <v>2</v>
       </c>
-      <c r="D34" s="45">
+      <c r="D34" s="44">
         <v>2</v>
       </c>
-      <c r="J34" s="47"/>
+      <c r="J34" s="46"/>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="46"/>
-      <c r="B35" s="44" t="s">
+      <c r="A35" s="45"/>
+      <c r="B35" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35" s="44">
+        <v>0</v>
+      </c>
+      <c r="J35" s="46"/>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="45"/>
+      <c r="B36" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-      <c r="D35" s="45">
-        <v>0</v>
-      </c>
-      <c r="J35" s="47"/>
-    </row>
-    <row r="36" spans="1:10">
-      <c r="A36" s="46"/>
-      <c r="B36" s="44" t="s">
-        <v>80</v>
-      </c>
       <c r="C36">
         <v>0</v>
       </c>
-      <c r="D36" s="45">
-        <v>0</v>
-      </c>
-      <c r="J36" s="47"/>
+      <c r="D36" s="44">
+        <v>0</v>
+      </c>
+      <c r="J36" s="46"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="46"/>
-      <c r="B37" s="49" t="s">
-        <v>78</v>
-      </c>
-      <c r="C37" s="44">
+      <c r="A37" s="45"/>
+      <c r="B37" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="43">
         <f>SUM(C32:C36)</f>
         <v>11</v>
       </c>
-      <c r="D37" s="48">
+      <c r="D37" s="47">
         <f>SUM(D32:D36)</f>
         <v>14.5</v>
       </c>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="50"/>
-      <c r="B38" s="51" t="s">
+      <c r="A38" s="49"/>
+      <c r="B38" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="52">
+      <c r="C38" s="51">
         <f>SUM(C7,C13,C19,C25,C31,C37)</f>
         <v>72</v>
       </c>
-      <c r="D38" s="53">
+      <c r="D38" s="52">
         <f>SUM(D7,D13,D19,D25,D31,D37)</f>
         <v>55</v>
       </c>

</xml_diff>